<commit_message>
Finally got the date selector working,
now I need to balance the Trial Balance Summary Report
</commit_message>
<xml_diff>
--- a/Reports/TrailBalanceSummary_001.xlsx
+++ b/Reports/TrailBalanceSummary_001.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Pagatech\Reports\"/>
@@ -15,21 +15,23 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Slicer_Hierarchy1">#N/A</definedName>
+    <definedName name="Slicer_MonthName">#N/A</definedName>
+    <definedName name="Slicer_YearNumber">#N/A</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId2"/>
+    <pivotCache cacheId="86" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
       <x14:pivotCaches>
-        <pivotCache cacheId="4" r:id="rId3"/>
+        <pivotCache cacheId="67" r:id="rId3"/>
       </x14:pivotCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
         <x14:slicerCache r:id="rId4"/>
+        <x14:slicerCache r:id="rId5"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -51,8 +53,37 @@
 </connections>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <metadataTypes count="1">
+    <metadataType name="XLMDX" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <metadataStrings count="3">
+    <s v="._SQL2012 AphelionPagaGLModel Model"/>
+    <s v="{[Shared_DimTransactionDate].[YearNumber].&amp;[2010],[Shared_DimTransactionDate].[YearNumber].&amp;[2011],[Shared_DimTransactionDate].[YearNumber].&amp;[2012],[Shared_DimTransactionDate].[YearNumber].&amp;[2013],[Shared_DimTransactionDate].[YearNumber].&amp;[2014]}"/>
+    <s v="{[Shared_DimTransactionDate].[MonthName].&amp;[May],[Shared_DimTransactionDate].[MonthName].&amp;[July],[Shared_DimTransactionDate].[MonthName].&amp;[June],[Shared_DimTransactionDate].[MonthName].&amp;[April],[Shared_DimTransactionDate].[MonthName].&amp;[March],[Shared_DimTransactionDate].[MonthName].&amp;[January],[Shared_DimTransactionDate].[MonthName].&amp;[February]}"/>
+  </metadataStrings>
+  <mdxMetadata count="2">
+    <mdx n="0" f="s">
+      <ms ns="1" c="0"/>
+    </mdx>
+    <mdx n="0" f="s">
+      <ms ns="2" c="0"/>
+    </mdx>
+  </mdxMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t>Row Labels</t>
   </si>
@@ -63,9 +94,6 @@
     <t>GLCreditAmount</t>
   </si>
   <si>
-    <t>GLBalance</t>
-  </si>
-  <si>
     <t>Assets</t>
   </si>
   <si>
@@ -117,6 +145,9 @@
     <t>Pool Accounts</t>
   </si>
   <si>
+    <t>Creditors - Airtime Stock Purchased</t>
+  </si>
+  <si>
     <t>Creditors - Cash Bonus Account</t>
   </si>
   <si>
@@ -138,6 +169,9 @@
     <t>Creditors - Transaction Processing Fees Payable</t>
   </si>
   <si>
+    <t>Creditors - VAT Payable</t>
+  </si>
+  <si>
     <t>Creditors - Virtual Account</t>
   </si>
   <si>
@@ -150,6 +184,9 @@
     <t>Creditors - Pagatech Airtime Sale Commission</t>
   </si>
   <si>
+    <t>Creditors - Pagatech Airtime Stock Repayment</t>
+  </si>
+  <si>
     <t>Creditors - Pagatech Bill Pay Commission</t>
   </si>
   <si>
@@ -174,6 +211,9 @@
     <t>Paga 3rd Party Funds Recievable</t>
   </si>
   <si>
+    <t>Stock - Airtime</t>
+  </si>
+  <si>
     <t>Debtors - Agent Accept Deposit Commission</t>
   </si>
   <si>
@@ -201,6 +241,9 @@
     <t>13110</t>
   </si>
   <si>
+    <t>21060</t>
+  </si>
+  <si>
     <t>21090</t>
   </si>
   <si>
@@ -222,6 +265,9 @@
     <t>21080</t>
   </si>
   <si>
+    <t>21050</t>
+  </si>
+  <si>
     <t>21020</t>
   </si>
   <si>
@@ -234,6 +280,9 @@
     <t>22020</t>
   </si>
   <si>
+    <t>22110</t>
+  </si>
+  <si>
     <t>22030</t>
   </si>
   <si>
@@ -258,6 +307,9 @@
     <t>12410</t>
   </si>
   <si>
+    <t>12490</t>
+  </si>
+  <si>
     <t>12110</t>
   </si>
   <si>
@@ -340,6 +392,24 @@
   </si>
   <si>
     <t>Paga - BFS Receivables</t>
+  </si>
+  <si>
+    <t>22060</t>
+  </si>
+  <si>
+    <t>Creditors - Pagatech Transaction History Fee</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>MonthName</t>
+  </si>
+  <si>
+    <t>YearNumber</t>
+  </si>
+  <si>
+    <t>(Multiple Items)</t>
   </si>
 </sst>
 </file>
@@ -407,21 +477,21 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Year"/>
+            <xdr:cNvPr id="4" name="YearNumber"/>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -430,12 +500,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Year"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="YearNumber"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -445,7 +515,79 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9525" y="190500"/>
+              <a:off x="0" y="190500"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="MonthName"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="MonthName"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="2905125"/>
               <a:ext cx="1828800" cy="2524125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -480,9 +622,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42055.413001504632" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42055.649045254628" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="12">
+  <cacheFields count="11">
     <cacheField name="[Classification_DimFinancialTransactionType].[SourceKey].[SourceKey]" caption="SourceKey" numFmtId="0" hierarchy="9" level="1">
       <sharedItems count="115">
         <s v="[Classification_DimFinancialTransactionType].[SourceKey].&amp;[AFFILIATE_AIRTIME_DISCOUNT_AWARD]" c="AFFILIATE_AIRTIME_DISCOUNT_AWARD"/>
@@ -602,24 +744,23 @@
         <s v="[Classification_DimFinancialTransactionType].[SourceKey].&amp;" c=""/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Measures].[GLDebitAmount]" caption="GLDebitAmount" numFmtId="0" hierarchy="361" level="32767"/>
-    <cacheField name="[Measures].[GLCreditAmount]" caption="GLCreditAmount" numFmtId="0" hierarchy="360" level="32767"/>
-    <cacheField name="[Measures].[GLBalance]" caption="GLBalance" numFmtId="0" hierarchy="362" level="32767"/>
-    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeGroup].[GLCodeGroup]" caption="GLCodeGroup" numFmtId="0" hierarchy="83" level="1">
+    <cacheField name="[Measures].[GLDebitAmount]" caption="GLDebitAmount" numFmtId="0" hierarchy="411" level="32767"/>
+    <cacheField name="[Measures].[GLCreditAmount]" caption="GLCreditAmount" numFmtId="0" hierarchy="410" level="32767"/>
+    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeGroup].[GLCodeGroup]" caption="GLCodeGroup" numFmtId="0" hierarchy="144" level="1">
       <sharedItems count="3">
         <s v="[Finance_GLCodeHierarchy].[GLCodeGroup].&amp;[Assets]" c="Assets"/>
         <s v="[Finance_GLCodeHierarchy].[GLCodeGroup].&amp;[Liabilities]" c="Liabilities"/>
         <s v="[Finance_GLCodeHierarchy].[GLCodeGroup].&amp;[Receivables]" c="Receivables"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeGroupRange].[GLCodeGroupRange]" caption="GLCodeGroupRange" numFmtId="0" hierarchy="84" level="1">
+    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeGroupRange].[GLCodeGroupRange]" caption="GLCodeGroupRange" numFmtId="0" hierarchy="145" level="1">
       <sharedItems count="3">
         <s v="[Finance_GLCodeHierarchy].[GLCodeGroupRange].&amp;[10100 - 19999]" c="10100 - 19999"/>
         <s v="[Finance_GLCodeHierarchy].[GLCodeGroupRange].&amp;[20000 - 29999]" c="20000 - 29999"/>
         <s v="[Finance_GLCodeHierarchy].[GLCodeGroupRange].&amp;[12000 - 12999]" c="12000 - 12999"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeSubGroup].[GLCodeSubGroup]" caption="GLCodeSubGroup" numFmtId="0" hierarchy="86" level="1">
+    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeSubGroup].[GLCodeSubGroup]" caption="GLCodeSubGroup" numFmtId="0" hierarchy="147" level="1">
       <sharedItems count="5">
         <s v="[Finance_GLCodeHierarchy].[GLCodeSubGroup].&amp;[Banks]" c="Banks"/>
         <s v="[Finance_GLCodeHierarchy].[GLCodeSubGroup].&amp;[Creditor Others]" c="Creditor Others"/>
@@ -628,7 +769,7 @@
         <s v="[Finance_GLCodeHierarchy].[GLCodeSubGroup].&amp;[Other Receivables]" c="Other Receivables"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeRange].[GLCodeRange]" caption="GLCodeRange" numFmtId="0" hierarchy="85" level="1">
+    <cacheField name="[Finance_GLCodeHierarchy].[GLCodeRange].[GLCodeRange]" caption="GLCodeRange" numFmtId="0" hierarchy="146" level="1">
       <sharedItems count="5">
         <s v="[Finance_GLCodeHierarchy].[GLCodeRange].&amp;[13000 - 13999]" c="13000 - 13999"/>
         <s v="[Finance_GLCodeHierarchy].[GLCodeRange].&amp;[21000 - 21299]" c="21000 - 21299"/>
@@ -637,13 +778,15 @@
         <s v="[Finance_GLCodeHierarchy].[GLCodeRange].&amp;[12400 - 12499]" c="12400 - 12499"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Finance_GLCodeHierarchy].[GLDescription].[GLDescription]" caption="GLDescription" numFmtId="0" hierarchy="87" level="1">
-      <sharedItems count="36">
+    <cacheField name="[Finance_GLCodeHierarchy].[GLDescription].[GLDescription]" caption="GLDescription" numFmtId="0" hierarchy="148" level="1">
+      <sharedItems count="41">
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Pool Accounts]" c="Pool Accounts"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Pre-Paid Service Repayment]" c="Creditors - Pagatech Pre-Paid Service Repayment"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Virtual Account]" c="Creditors - Virtual Account"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Commission Payable]" c="Creditors - Commission Payable"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Commission Accrued]" c="Creditors - Commission Accrued"/>
+        <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - VAT Payable]" c="Creditors - VAT Payable"/>
+        <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Airtime Stock Purchased]" c="Creditors - Airtime Stock Purchased"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Transaction Processing Fees Payable]" c="Creditors - Transaction Processing Fees Payable"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Cash Bonus Account]" c="Creditors - Cash Bonus Account"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech BFS Payables]" c="Creditors - Pagatech BFS Payables"/>
@@ -656,9 +799,11 @@
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Bill Pay Commission]" c="Creditors - Pagatech Bill Pay Commission"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Merchant Transaction Fees]" c="Creditors - Pagatech Merchant Transaction Fees"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Account Balance Fee]" c="Creditors - Pagatech Account Balance Fee"/>
+        <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Transaction History Fee]" c="Creditors - Pagatech Transaction History Fee"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Withdrawals Fee]" c="Creditors - Pagatech Withdrawals Fee"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Load Cash Fee]" c="Creditors - Pagatech Load Cash Fee"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Premium SMS Fee]" c="Creditors - Pagatech Premium SMS Fee"/>
+        <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Pagatech Airtime Stock Repayment]" c="Creditors - Pagatech Airtime Stock Repayment"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Creditors - Fees Accrued]" c="Creditors - Fees Accrued"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Debtors - Agent Accept Deposit Commission]" c="Debtors - Agent Accept Deposit Commission"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Debtors - Agent Sign up Fees Commission]" c="Debtors - Agent Sign up Fees Commission"/>
@@ -675,15 +820,18 @@
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Debtors - Merchant Stock]" c="Debtors - Merchant Stock"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Paga 3rd Party Funds Recievable]" c="Paga 3rd Party Funds Recievable"/>
         <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Paga - BFS Receivables]" c="Paga - BFS Receivables"/>
+        <s v="[Finance_GLCodeHierarchy].[GLDescription].&amp;[Stock - Airtime]" c="Stock - Airtime"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Finance_GLCodeHierarchy].[GLCode].[GLCode]" caption="GLCode" numFmtId="0" hierarchy="82" level="1">
-      <sharedItems count="36">
+    <cacheField name="[Finance_GLCodeHierarchy].[GLCode].[GLCode]" caption="GLCode" numFmtId="0" hierarchy="143" level="1">
+      <sharedItems count="41">
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[13110]" c="13110"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21010]" c="21010"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21020]" c="21020"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21030]" c="21030"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21040]" c="21040"/>
+        <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21050]" c="21050"/>
+        <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21060]" c="21060"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21080]" c="21080"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21090]" c="21090"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[21100]" c="21100"/>
@@ -696,9 +844,11 @@
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22030]" c="22030"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22040]" c="22040"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22050]" c="22050"/>
+        <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22060]" c="22060"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22070]" c="22070"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22080]" c="22080"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22090]" c="22090"/>
+        <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22110]" c="22110"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[22120]" c="22120"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[12110]" c="12110"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[12120]" c="12120"/>
@@ -715,16 +865,17 @@
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[12230]" c="12230"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[12410]" c="12410"/>
         <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[12430]" c="12430"/>
+        <s v="[Finance_GLCodeHierarchy].[GLCode].&amp;[12490]" c="12490"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Shared_DimTransactionDate].[Hierarchy1].[Year]" caption="Year" numFmtId="0" hierarchy="238" level="1">
+    <cacheField name="[Shared_DimTransactionDate].[MonthName].[MonthName]" caption="MonthName" numFmtId="0" hierarchy="286" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
-    <cacheField name="[Shared_DimTransactionDate].[Hierarchy1].[MonthName]" caption="MonthName" numFmtId="0" hierarchy="238" level="2">
+    <cacheField name="[Shared_DimTransactionDate].[YearNumber].[YearNumber]" caption="YearNumber" numFmtId="0" hierarchy="296" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="396">
+  <cacheHierarchies count="455">
     <cacheHierarchy uniqueName="[Classification_DimAgentCommissionType].[DimAgentCommissionTypeID]" caption="DimAgentCommissionTypeID" attribute="1" defaultMemberUniqueName="[Classification_DimAgentCommissionType].[DimAgentCommissionTypeID].[All]" allUniqueName="[Classification_DimAgentCommissionType].[DimAgentCommissionTypeID].[All]" dimensionUniqueName="[Classification_DimAgentCommissionType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimAgentCommissionType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Classification_DimAgentCommissionType].[Name].[All]" allUniqueName="[Classification_DimAgentCommissionType].[Name].[All]" dimensionUniqueName="[Classification_DimAgentCommissionType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimAgentCommissionType].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Classification_DimAgentCommissionType].[SourceKey].[All]" allUniqueName="[Classification_DimAgentCommissionType].[SourceKey].[All]" dimensionUniqueName="[Classification_DimAgentCommissionType]" displayFolder="" count="0" unbalanced="0"/>
@@ -760,6 +911,66 @@
     <cacheHierarchy uniqueName="[Classification_DimProcessType].[DimProcessTypeID]" caption="DimProcessTypeID" attribute="1" defaultMemberUniqueName="[Classification_DimProcessType].[DimProcessTypeID].[All]" allUniqueName="[Classification_DimProcessType].[DimProcessTypeID].[All]" dimensionUniqueName="[Classification_DimProcessType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimProcessType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Classification_DimProcessType].[Name].[All]" allUniqueName="[Classification_DimProcessType].[Name].[All]" dimensionUniqueName="[Classification_DimProcessType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimProcessType].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Classification_DimProcessType].[SourceKey].[All]" allUniqueName="[Classification_DimProcessType].[SourceKey].[All]" dimensionUniqueName="[Classification_DimProcessType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[Aggregate]" caption="Aggregate" attribute="1" defaultMemberUniqueName="[DatePeriods].[Aggregate].[All]" allUniqueName="[DatePeriods].[Aggregate].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[Number]" caption="Number" attribute="1" defaultMemberUniqueName="[DatePeriods].[Number].[All]" allUniqueName="[DatePeriods].[Number].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[OrderNumber]" caption="OrderNumber" attribute="1" defaultMemberUniqueName="[DatePeriods].[OrderNumber].[All]" allUniqueName="[DatePeriods].[OrderNumber].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[Period]" caption="Period" attribute="1" defaultMemberUniqueName="[DatePeriods].[Period].[All]" allUniqueName="[DatePeriods].[Period].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[PeriodName]" caption="PeriodName" attribute="1" defaultMemberUniqueName="[DatePeriods].[PeriodName].[All]" allUniqueName="[DatePeriods].[PeriodName].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[PeriodType]" caption="PeriodType" attribute="1" defaultMemberUniqueName="[DatePeriods].[PeriodType].[All]" allUniqueName="[DatePeriods].[PeriodType].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[Date].[All]" allUniqueName="[DatePeriodSelector].[Date].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DateID].[All]" allUniqueName="[DatePeriodSelector].[DateID].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DateSK].[All]" allUniqueName="[DatePeriodSelector].[DateSK].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[Day].[All]" allUniqueName="[DatePeriodSelector].[Day].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DayOfWeek].[All]" allUniqueName="[DatePeriodSelector].[DayOfWeek].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DayOfYear].[All]" allUniqueName="[DatePeriodSelector].[DayOfYear].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DaySuffix].[All]" allUniqueName="[DatePeriodSelector].[DaySuffix].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DOWInMonth].[All]" allUniqueName="[DatePeriodSelector].[DOWInMonth].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialPeriodAllTime].[All]" allUniqueName="[DatePeriodSelector].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialPeriodName].[All]" allUniqueName="[DatePeriodSelector].[FinancialPeriodName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialPeriodNumber].[All]" allUniqueName="[DatePeriodSelector].[FinancialPeriodNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialYearName].[All]" allUniqueName="[DatePeriodSelector].[FinancialYearName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialYearNumber].[All]" allUniqueName="[DatePeriodSelector].[FinancialYearNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[HolidayText].[All]" allUniqueName="[DatePeriodSelector].[HolidayText].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[IsPublicHoliday].[All]" allUniqueName="[DatePeriodSelector].[IsPublicHoliday].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[MonthAllTime].[All]" allUniqueName="[DatePeriodSelector].[MonthAllTime].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[MonthName].[All]" allUniqueName="[DatePeriodSelector].[MonthName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[MonthNumber].[All]" allUniqueName="[DatePeriodSelector].[MonthNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[Quarter].[All]" allUniqueName="[DatePeriodSelector].[Quarter].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[QuarterAllTime].[All]" allUniqueName="[DatePeriodSelector].[QuarterAllTime].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[QuarterName].[All]" allUniqueName="[DatePeriodSelector].[QuarterName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[StandardDate].[All]" allUniqueName="[DatePeriodSelector].[StandardDate].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[USDayOfWeek].[All]" allUniqueName="[DatePeriodSelector].[USDayOfWeek].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[WeekOfMonth].[All]" allUniqueName="[DatePeriodSelector].[WeekOfMonth].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[WeekOfYear].[All]" allUniqueName="[DatePeriodSelector].[WeekOfYear].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[YearName].[All]" allUniqueName="[DatePeriodSelector].[YearName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[YearNumber].[All]" allUniqueName="[DatePeriodSelector].[YearNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[DimDate].[Date].[All]" allUniqueName="[DimDate].[Date].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[DimDate].[DateID].[All]" allUniqueName="[DimDate].[DateID].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[DimDate].[DateSK].[All]" allUniqueName="[DimDate].[DateSK].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[DimDate].[Day].[All]" allUniqueName="[DimDate].[Day].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[DimDate].[DayOfWeek].[All]" allUniqueName="[DimDate].[DayOfWeek].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[DimDate].[DayOfYear].[All]" allUniqueName="[DimDate].[DayOfYear].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[DimDate].[DaySuffix].[All]" allUniqueName="[DimDate].[DaySuffix].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[DimDate].[DOWInMonth].[All]" allUniqueName="[DimDate].[DOWInMonth].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialPeriodAllTime].[All]" allUniqueName="[DimDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialPeriodName].[All]" allUniqueName="[DimDate].[FinancialPeriodName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialPeriodNumber].[All]" allUniqueName="[DimDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialYearName].[All]" allUniqueName="[DimDate].[FinancialYearName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialYearNumber].[All]" allUniqueName="[DimDate].[FinancialYearNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[DimDate].[HolidayText].[All]" allUniqueName="[DimDate].[HolidayText].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[DimDate].[IsPublicHoliday].[All]" allUniqueName="[DimDate].[IsPublicHoliday].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[DimDate].[MonthAllTime].[All]" allUniqueName="[DimDate].[MonthAllTime].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[DimDate].[MonthName].[All]" allUniqueName="[DimDate].[MonthName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[DimDate].[MonthNumber].[All]" allUniqueName="[DimDate].[MonthNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[DimDate].[Quarter].[All]" allUniqueName="[DimDate].[Quarter].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[DimDate].[QuarterAllTime].[All]" allUniqueName="[DimDate].[QuarterAllTime].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[DimDate].[QuarterName].[All]" allUniqueName="[DimDate].[QuarterName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[DimDate].[StandardDate].[All]" allUniqueName="[DimDate].[StandardDate].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[DimDate].[USDayOfWeek].[All]" allUniqueName="[DimDate].[USDayOfWeek].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[DimDate].[WeekOfMonth].[All]" allUniqueName="[DimDate].[WeekOfMonth].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[DimDate].[WeekOfYear].[All]" allUniqueName="[DimDate].[WeekOfYear].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[DimDate].[YearName].[All]" allUniqueName="[DimDate].[YearName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[DimDate].[YearNumber].[All]" allUniqueName="[DimDate].[YearNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_ChartOfAccounts].[COA_CodeRange]" caption="COA_CodeRange" attribute="1" defaultMemberUniqueName="[Finance_ChartOfAccounts].[COA_CodeRange].[All]" allUniqueName="[Finance_ChartOfAccounts].[COA_CodeRange].[All]" dimensionUniqueName="[Finance_ChartOfAccounts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_ChartOfAccounts].[COA_Name]" caption="COA_Name" attribute="1" defaultMemberUniqueName="[Finance_ChartOfAccounts].[COA_Name].[All]" allUniqueName="[Finance_ChartOfAccounts].[COA_Name].[All]" dimensionUniqueName="[Finance_ChartOfAccounts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_ChartOfAccounts].[DimChartOfAccountsID]" caption="DimChartOfAccountsID" attribute="1" defaultMemberUniqueName="[Finance_ChartOfAccounts].[DimChartOfAccountsID].[All]" allUniqueName="[Finance_ChartOfAccounts].[DimChartOfAccountsID].[All]" dimensionUniqueName="[Finance_ChartOfAccounts]" displayFolder="" count="0" unbalanced="0"/>
@@ -767,9 +978,9 @@
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimBankAccountID]" caption="DimBankAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimBankAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimBankAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimCurrencyID]" caption="DimCurrencyID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimCurrencyID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimCurrencyID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountID]" caption="DimFinancialAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountTypeID]" caption="DimFinancialAccountTypeID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountTypeID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountTypeID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimFinancialHoldingAccountID]" caption="DimFinancialHoldingAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimFinancialHoldingAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimFinancialHoldingAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimPagaAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimPagaAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[FinancialAccountType]" caption="FinancialAccountType" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[FinancialAccountType].[All]" allUniqueName="[Finance_DimFinancialAccount].[FinancialAccountType].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[Name].[All]" allUniqueName="[Finance_DimFinancialAccount].[Name].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[OpeningBalance]" caption="OpeningBalance" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[OpeningBalance].[All]" allUniqueName="[Finance_DimFinancialAccount].[OpeningBalance].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[RestrictedBalance].[All]" allUniqueName="[Finance_DimFinancialAccount].[RestrictedBalance].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
@@ -799,11 +1010,12 @@
     <cacheHierarchy uniqueName="[Finance_FactFinancialTransaction].[ShortCode]" caption="ShortCode" attribute="1" defaultMemberUniqueName="[Finance_FactFinancialTransaction].[ShortCode].[All]" allUniqueName="[Finance_FactFinancialTransaction].[ShortCode].[All]" dimensionUniqueName="[Finance_FactFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactFinancialTransaction].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Finance_FactFinancialTransaction].[SourceKey].[All]" allUniqueName="[Finance_FactFinancialTransaction].[SourceKey].[All]" dimensionUniqueName="[Finance_FactFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactFinancialTransaction].[TextDescription]" caption="TextDescription" attribute="1" defaultMemberUniqueName="[Finance_FactFinancialTransaction].[TextDescription].[All]" allUniqueName="[Finance_FactFinancialTransaction].[TextDescription].[All]" dimensionUniqueName="[Finance_FactFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[Balance]" caption="Balance" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[Balance].[All]" allUniqueName="[Finance_FactGLTransaction].[Balance].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[CreditAmount]" caption="CreditAmount" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[CreditAmount].[All]" allUniqueName="[Finance_FactGLTransaction].[CreditAmount].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[DebitAmount]" caption="DebitAmount" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[DebitAmount].[All]" allUniqueName="[Finance_FactGLTransaction].[DebitAmount].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[DimFinancialAccountID]" caption="DimFinancialAccountID" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[DimFinancialAccountID].[All]" allUniqueName="[Finance_FactGLTransaction].[DimFinancialAccountID].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[DimGLCodeID]" caption="DimGLCodeID" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[DimGLCodeID].[All]" allUniqueName="[Finance_FactGLTransaction].[DimGLCodeID].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[DimTransactionDateID]" caption="DimTransactionDateID" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[DimTransactionDateID].[All]" allUniqueName="[Finance_FactGLTransaction].[DimTransactionDateID].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[DimTransactionDateID]" caption="DimTransactionDateID" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[DimTransactionDateID].[All]" allUniqueName="[Finance_FactGLTransaction].[DimTransactionDateID].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="2" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[FactFinancialTxID]" caption="FactFinancialTxID" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[FactFinancialTxID].[All]" allUniqueName="[Finance_FactGLTransaction].[FactFinancialTxID].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[FactGLTxID]" caption="FactGLTxID" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[FactGLTxID].[All]" allUniqueName="[Finance_FactGLTransaction].[FactGLTxID].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[Movement]" caption="Movement" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[Movement].[All]" allUniqueName="[Finance_FactGLTransaction].[Movement].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
@@ -815,37 +1027,37 @@
     <cacheHierarchy uniqueName="[Finance_GLCodeHierarchy].[GLCode]" caption="GLCode" attribute="1" defaultMemberUniqueName="[Finance_GLCodeHierarchy].[GLCode].[All]" allUniqueName="[Finance_GLCodeHierarchy].[GLCode].[All]" dimensionUniqueName="[Finance_GLCodeHierarchy]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="9"/>
+        <fieldUsage x="8"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Finance_GLCodeHierarchy].[GLCodeGroup]" caption="GLCodeGroup" attribute="1" defaultMemberUniqueName="[Finance_GLCodeHierarchy].[GLCodeGroup].[All]" allUniqueName="[Finance_GLCodeHierarchy].[GLCodeGroup].[All]" dimensionUniqueName="[Finance_GLCodeHierarchy]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="4"/>
+        <fieldUsage x="3"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Finance_GLCodeHierarchy].[GLCodeGroupRange]" caption="GLCodeGroupRange" attribute="1" defaultMemberUniqueName="[Finance_GLCodeHierarchy].[GLCodeGroupRange].[All]" allUniqueName="[Finance_GLCodeHierarchy].[GLCodeGroupRange].[All]" dimensionUniqueName="[Finance_GLCodeHierarchy]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="5"/>
+        <fieldUsage x="4"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Finance_GLCodeHierarchy].[GLCodeRange]" caption="GLCodeRange" attribute="1" defaultMemberUniqueName="[Finance_GLCodeHierarchy].[GLCodeRange].[All]" allUniqueName="[Finance_GLCodeHierarchy].[GLCodeRange].[All]" dimensionUniqueName="[Finance_GLCodeHierarchy]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="7"/>
+        <fieldUsage x="6"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Finance_GLCodeHierarchy].[GLCodeSubGroup]" caption="GLCodeSubGroup" attribute="1" defaultMemberUniqueName="[Finance_GLCodeHierarchy].[GLCodeSubGroup].[All]" allUniqueName="[Finance_GLCodeHierarchy].[GLCodeSubGroup].[All]" dimensionUniqueName="[Finance_GLCodeHierarchy]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="6"/>
+        <fieldUsage x="5"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Finance_GLCodeHierarchy].[GLDescription]" caption="GLDescription" attribute="1" defaultMemberUniqueName="[Finance_GLCodeHierarchy].[GLDescription].[All]" allUniqueName="[Finance_GLCodeHierarchy].[GLDescription].[All]" dimensionUniqueName="[Finance_GLCodeHierarchy]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="8"/>
+        <fieldUsage x="7"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Shared_DimApprovingUser].[DimApprovingUser]" caption="DimApprovingUser" attribute="1" defaultMemberUniqueName="[Shared_DimApprovingUser].[DimApprovingUser].[All]" allUniqueName="[Shared_DimApprovingUser].[DimApprovingUser].[All]" dimensionUniqueName="[Shared_DimApprovingUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -874,32 +1086,33 @@
     <cacheHierarchy uniqueName="[Shared_DimCancellingUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Shared_DimCancellingUser].[Name].[All]" allUniqueName="[Shared_DimCancellingUser].[Name].[All]" dimensionUniqueName="[Shared_DimCancellingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimCancellingUser].[PhoneNumber]" caption="PhoneNumber" attribute="1" defaultMemberUniqueName="[Shared_DimCancellingUser].[PhoneNumber].[All]" allUniqueName="[Shared_DimCancellingUser].[PhoneNumber].[All]" dimensionUniqueName="[Shared_DimCancellingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimCancellingUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimCancellingUser].[SourceKey].[All]" allUniqueName="[Shared_DimCancellingUser].[SourceKey].[All]" dimensionUniqueName="[Shared_DimCancellingUser]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DayName].[All]" allUniqueName="[Shared_DimCompletedDate].[DayName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimCompletedDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DayOfYear].[All]" allUniqueName="[Shared_DimCompletedDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DimCompletedDateID]" caption="DimCompletedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DimCompletedDateID].[All]" allUniqueName="[Shared_DimCompletedDate].[DimCompletedDateID].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[FullDate].[All]" allUniqueName="[Shared_DimCompletedDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[MMYYYY].[All]" allUniqueName="[Shared_DimCompletedDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[Month].[All]" allUniqueName="[Shared_DimCompletedDate].[Month].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[MonthName].[All]" allUniqueName="[Shared_DimCompletedDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[MonthYear].[All]" allUniqueName="[Shared_DimCompletedDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[Quarter].[All]" allUniqueName="[Shared_DimCompletedDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[QuarterName].[All]" allUniqueName="[Shared_DimCompletedDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[Year].[All]" allUniqueName="[Shared_DimCompletedDate].[Year].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[YearName].[All]" allUniqueName="[Shared_DimCompletedDate].[YearName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayName].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Date].[All]" allUniqueName="[Shared_DimEffectiveDate].[Date].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DateID].[All]" allUniqueName="[Shared_DimEffectiveDate].[DateID].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DateSK].[All]" allUniqueName="[Shared_DimEffectiveDate].[DateSK].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Day].[All]" allUniqueName="[Shared_DimEffectiveDate].[Day].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayOfWeek].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayOfWeek].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayOfYear].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DimEffectiveDateID]" caption="DimEffectiveDateID" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DimEffectiveDateID].[All]" allUniqueName="[Shared_DimEffectiveDate].[DimEffectiveDateID].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FullDate].[All]" allUniqueName="[Shared_DimEffectiveDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MMYYYY].[All]" allUniqueName="[Shared_DimEffectiveDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Month].[All]" allUniqueName="[Shared_DimEffectiveDate].[Month].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DaySuffix].[All]" allUniqueName="[Shared_DimEffectiveDate].[DaySuffix].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DOWInMonth].[All]" allUniqueName="[Shared_DimEffectiveDate].[DOWInMonth].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodAllTime].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodName].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialYearName].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialYearName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialYearNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialYearNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[HolidayText].[All]" allUniqueName="[Shared_DimEffectiveDate].[HolidayText].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[IsPublicHoliday].[All]" allUniqueName="[Shared_DimEffectiveDate].[IsPublicHoliday].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthAllTime].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthAllTime].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthName].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthYear].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Quarter].[All]" allUniqueName="[Shared_DimEffectiveDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[QuarterAllTime].[All]" allUniqueName="[Shared_DimEffectiveDate].[QuarterAllTime].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[QuarterName].[All]" allUniqueName="[Shared_DimEffectiveDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Year].[All]" allUniqueName="[Shared_DimEffectiveDate].[Year].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[StandardDate].[All]" allUniqueName="[Shared_DimEffectiveDate].[StandardDate].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[USDayOfWeek].[All]" allUniqueName="[Shared_DimEffectiveDate].[USDayOfWeek].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[WeekOfMonth].[All]" allUniqueName="[Shared_DimEffectiveDate].[WeekOfMonth].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[WeekOfYear].[All]" allUniqueName="[Shared_DimEffectiveDate].[WeekOfYear].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[YearName].[All]" allUniqueName="[Shared_DimEffectiveDate].[YearName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[YearNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[YearNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimForUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimForUser].[DimCreatedDateID].[All]" allUniqueName="[Shared_DimForUser].[DimCreatedDateID].[All]" dimensionUniqueName="[Shared_DimForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimForUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[Shared_DimForUser].[DimDateOfBirthID].[All]" allUniqueName="[Shared_DimForUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[Shared_DimForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimForUser].[DimForUserID]" caption="DimForUserID" attribute="1" defaultMemberUniqueName="[Shared_DimForUser].[DimForUserID].[All]" allUniqueName="[Shared_DimForUser].[DimForUserID].[All]" dimensionUniqueName="[Shared_DimForUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -926,19 +1139,6 @@
     <cacheHierarchy uniqueName="[Shared_DimInitiatingUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Shared_DimInitiatingUser].[Name].[All]" allUniqueName="[Shared_DimInitiatingUser].[Name].[All]" dimensionUniqueName="[Shared_DimInitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimInitiatingUser].[PhoneNumber]" caption="PhoneNumber" attribute="1" defaultMemberUniqueName="[Shared_DimInitiatingUser].[PhoneNumber].[All]" allUniqueName="[Shared_DimInitiatingUser].[PhoneNumber].[All]" dimensionUniqueName="[Shared_DimInitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimInitiatingUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimInitiatingUser].[SourceKey].[All]" allUniqueName="[Shared_DimInitiatingUser].[SourceKey].[All]" dimensionUniqueName="[Shared_DimInitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DayName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DayName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DayOfYear].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DimIntegrationTxDateID]" caption="DimIntegrationTxDateID" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DimIntegrationTxDateID].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DimIntegrationTxDateID].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[FullDate].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[MMYYYY].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[Month].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[Month].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[MonthName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[MonthYear].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[Quarter].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[QuarterName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[Year].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[Year].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[YearName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[YearName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimPagaAccount].[BankingStatus]" caption="BankingStatus" attribute="1" defaultMemberUniqueName="[Shared_DimPagaAccount].[BankingStatus].[All]" allUniqueName="[Shared_DimPagaAccount].[BankingStatus].[All]" dimensionUniqueName="[Shared_DimPagaAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimPagaAccount].[CreatedDateID]" caption="CreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimPagaAccount].[CreatedDateID].[All]" allUniqueName="[Shared_DimPagaAccount].[CreatedDateID].[All]" dimensionUniqueName="[Shared_DimPagaAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimPagaAccount].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[Shared_DimPagaAccount].[DimPagaAccountID].[All]" allUniqueName="[Shared_DimPagaAccount].[DimPagaAccountID].[All]" dimensionUniqueName="[Shared_DimPagaAccount]" displayFolder="" count="0" unbalanced="0"/>
@@ -968,19 +1168,6 @@
     <cacheHierarchy uniqueName="[Shared_DimRole].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimRole].[SourceKey].[All]" allUniqueName="[Shared_DimRole].[SourceKey].[All]" dimensionUniqueName="[Shared_DimRole]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimRole].[SystemDescription]" caption="SystemDescription" attribute="1" defaultMemberUniqueName="[Shared_DimRole].[SystemDescription].[All]" allUniqueName="[Shared_DimRole].[SystemDescription].[All]" dimensionUniqueName="[Shared_DimRole]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimRole].[TextDesciption]" caption="TextDesciption" attribute="1" defaultMemberUniqueName="[Shared_DimRole].[TextDesciption].[All]" allUniqueName="[Shared_DimRole].[TextDesciption].[All]" dimensionUniqueName="[Shared_DimRole]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DayName].[All]" allUniqueName="[Shared_DimStartedDate].[DayName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimStartedDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DayOfYear].[All]" allUniqueName="[Shared_DimStartedDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DimStartedDateID]" caption="DimStartedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DimStartedDateID].[All]" allUniqueName="[Shared_DimStartedDate].[DimStartedDateID].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[FullDate].[All]" allUniqueName="[Shared_DimStartedDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[MMYYYY].[All]" allUniqueName="[Shared_DimStartedDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[Month].[All]" allUniqueName="[Shared_DimStartedDate].[Month].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[MonthName].[All]" allUniqueName="[Shared_DimStartedDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[MonthYear].[All]" allUniqueName="[Shared_DimStartedDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[Quarter].[All]" allUniqueName="[Shared_DimStartedDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[QuarterName].[All]" allUniqueName="[Shared_DimStartedDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[Year].[All]" allUniqueName="[Shared_DimStartedDate].[Year].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[YearName].[All]" allUniqueName="[Shared_DimStartedDate].[YearName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[DimCreatedDateID].[All]" allUniqueName="[Shared_DimToUser].[DimCreatedDateID].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[DimDateOfBirthID].[All]" allUniqueName="[Shared_DimToUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[DimPrimaryRoleID]" caption="DimPrimaryRoleID" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[DimPrimaryRoleID].[All]" allUniqueName="[Shared_DimToUser].[DimPrimaryRoleID].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -994,25 +1181,43 @@
     <cacheHierarchy uniqueName="[Shared_DimToUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[Name].[All]" allUniqueName="[Shared_DimToUser].[Name].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[PhoneNumber]" caption="PhoneNumber" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[PhoneNumber].[All]" allUniqueName="[Shared_DimToUser].[PhoneNumber].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[SourceKey].[All]" allUniqueName="[Shared_DimToUser].[SourceKey].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayName].[All]" allUniqueName="[Shared_DimTransactionDate].[DayName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimTransactionDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DimTransactionDateID]" caption="DimTransactionDateID" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DimTransactionDateID].[All]" allUniqueName="[Shared_DimTransactionDate].[DimTransactionDateID].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FullDate].[All]" allUniqueName="[Shared_DimTransactionDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Hierarchy1]" caption="Hierarchy1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Hierarchy1].[All]" allUniqueName="[Shared_DimTransactionDate].[Hierarchy1].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="3" unbalanced="0">
-      <fieldsUsage count="3">
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Date].[All]" allUniqueName="[Shared_DimTransactionDate].[Date].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DateID].[All]" allUniqueName="[Shared_DimTransactionDate].[DateID].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DateSK].[All]" allUniqueName="[Shared_DimTransactionDate].[DateSK].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Day].[All]" allUniqueName="[Shared_DimTransactionDate].[Day].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayOfWeek].[All]" allUniqueName="[Shared_DimTransactionDate].[DayOfWeek].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayOfYear].[All]" allUniqueName="[Shared_DimTransactionDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DaySuffix].[All]" allUniqueName="[Shared_DimTransactionDate].[DaySuffix].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DOWInMonth].[All]" allUniqueName="[Shared_DimTransactionDate].[DOWInMonth].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialPeriodAllTime].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialPeriodName].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialPeriodName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialPeriodNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialYearName].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialYearName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialYearNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialYearNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[HolidayText].[All]" allUniqueName="[Shared_DimTransactionDate].[HolidayText].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[IsPublicHoliday].[All]" allUniqueName="[Shared_DimTransactionDate].[IsPublicHoliday].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthAllTime].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthAllTime].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthName].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="9"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Quarter].[All]" allUniqueName="[Shared_DimTransactionDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[QuarterAllTime].[All]" allUniqueName="[Shared_DimTransactionDate].[QuarterAllTime].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[QuarterName].[All]" allUniqueName="[Shared_DimTransactionDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[StandardDate].[All]" allUniqueName="[Shared_DimTransactionDate].[StandardDate].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[USDayOfWeek].[All]" allUniqueName="[Shared_DimTransactionDate].[USDayOfWeek].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[WeekOfMonth].[All]" allUniqueName="[Shared_DimTransactionDate].[WeekOfMonth].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[WeekOfYear].[All]" allUniqueName="[Shared_DimTransactionDate].[WeekOfYear].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[YearName].[All]" allUniqueName="[Shared_DimTransactionDate].[YearName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[YearNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[YearNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
         <fieldUsage x="-1"/>
         <fieldUsage x="10"/>
-        <fieldUsage x="11"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MMYYYY].[All]" allUniqueName="[Shared_DimTransactionDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Month].[All]" allUniqueName="[Shared_DimTransactionDate].[Month].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthName].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthYear].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Quarter].[All]" allUniqueName="[Shared_DimTransactionDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[QuarterName].[All]" allUniqueName="[Shared_DimTransactionDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Year].[All]" allUniqueName="[Shared_DimTransactionDate].[Year].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[YearName].[All]" allUniqueName="[Shared_DimTransactionDate].[YearName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimUser].[DimCreatedDateID].[All]" allUniqueName="[Shared_DimUser].[DimCreatedDateID].[All]" dimensionUniqueName="[Shared_DimUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[Shared_DimUser].[DimDateOfBirthID].[All]" allUniqueName="[Shared_DimUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[Shared_DimUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimUser].[DimPrimaryRoleID]" caption="DimPrimaryRoleID" attribute="1" defaultMemberUniqueName="[Shared_DimUser].[DimPrimaryRoleID].[All]" allUniqueName="[Shared_DimUser].[DimPrimaryRoleID].[All]" dimensionUniqueName="[Shared_DimUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -1107,23 +1312,23 @@
     <cacheHierarchy uniqueName="[Shared_Organization].[TextDesciption]" caption="TextDesciption" attribute="1" defaultMemberUniqueName="[Shared_Organization].[TextDesciption].[All]" allUniqueName="[Shared_Organization].[TextDesciption].[All]" dimensionUniqueName="[Shared_Organization]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_Organization].[VATCertificationNumber]" caption="VATCertificationNumber" attribute="1" defaultMemberUniqueName="[Shared_Organization].[VATCertificationNumber].[All]" allUniqueName="[Shared_Organization].[VATCertificationNumber].[All]" dimensionUniqueName="[Shared_Organization]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_Organization].[WebsiteURL]" caption="WebsiteURL" attribute="1" defaultMemberUniqueName="[Shared_Organization].[WebsiteURL].[All]" allUniqueName="[Shared_Organization].[WebsiteURL].[All]" dimensionUniqueName="[Shared_Organization]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationID]" caption="DimOrganizationID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel1ID]" caption="DimOrganizationUnitLevel1ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel1ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel1ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel2ID]" caption="DimOrganizationUnitLevel2ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel2ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel2ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel3ID]" caption="DimOrganizationUnitLevel3ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel3ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel3ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel4ID]" caption="DimOrganizationUnitLevel4ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel4ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel4ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1]" caption="OrgLevel1" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_IdentificationNumber]" caption="OrgLevel1_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_UnitType]" caption="OrgLevel1_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2]" caption="OrgLevel2" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_IdentificationNumber]" caption="OrgLevel2_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_UnitType]" caption="OrgLevel2_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3]" caption="OrgLevel3" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_IdentificationNumber]" caption="OrgLevel3_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_UnitType]" caption="OrgLevel3_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4]" caption="OrgLevel4" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_IdentificationNumber]" caption="OrgLevel4_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_UnitType]" caption="OrgLevel4_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationID]" caption="DimOrganizationID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel1ID]" caption="DimOrganizationUnitLevel1ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel1ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel1ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel2ID]" caption="DimOrganizationUnitLevel2ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel2ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel2ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel3ID]" caption="DimOrganizationUnitLevel3ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel3ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel3ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel4ID]" caption="DimOrganizationUnitLevel4ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel4ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel4ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1]" caption="OrgLevel1" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_IdentificationNumber]" caption="OrgLevel1_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_UnitType]" caption="OrgLevel1_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2]" caption="OrgLevel2" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_IdentificationNumber]" caption="OrgLevel2_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_UnitType]" caption="OrgLevel2_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3]" caption="OrgLevel3" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_IdentificationNumber]" caption="OrgLevel3_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_UnitType]" caption="OrgLevel3_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4]" caption="OrgLevel4" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_IdentificationNumber]" caption="OrgLevel4_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_UnitType]" caption="OrgLevel4_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[TransactionCount]" caption="TransactionCount" measure="1" displayFolder="" measureGroup="Finance_FactFinancialTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[TransactionAmount]" caption="TransactionAmount" measure="1" displayFolder="" measureGroup="Finance_FactFinancialTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[GLCreditAmount]" caption="GLCreditAmount" measure="1" displayFolder="" measureGroup="Finance_FactGLTransaction" count="0" oneField="1">
@@ -1136,11 +1341,16 @@
         <fieldUsage x="1"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[GLBalance]" caption="GLBalance" measure="1" displayFolder="" measureGroup="Finance_FactGLTransaction" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="3"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[PeriodValue]" caption="PeriodValue" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[PeriodNumber]" caption="PeriodNumber" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[PeriodAggregate]" caption="PeriodAggregate" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[PeriodTypeVal]" caption="PeriodTypeVal" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[FilterStartDateID]" caption="FilterStartDateID" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[FilterEndDateID]" caption="FilterEndDateID" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Minimum of MonthNumber]" caption="Minimum of MonthNumber" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Maximum of MonthNumber]" caption="Maximum of MonthNumber" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[MinDate]" caption="MinDate" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[MaxDate]" caption="MaxDate" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_FactFinancialTransaction]" caption="_Count Finance_FactFinancialTransaction" measure="1" displayFolder="" measureGroup="Finance_FactFinancialTransaction" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_FactGLTransaction]" caption="_Count Finance_FactGLTransaction" measure="1" displayFolder="" measureGroup="Finance_FactGLTransaction" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimRole]" caption="_Count Shared_DimRole" measure="1" displayFolder="" measureGroup="Shared_DimRole" count="0" hidden="1"/>
@@ -1165,14 +1375,14 @@
     <cacheHierarchy uniqueName="[Measures].[_Count Classification_DimProcessType]" caption="_Count Classification_DimProcessType" measure="1" displayFolder="" measureGroup="Classification_DimProcessType" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimPagaAccount]" caption="_Count Shared_DimPagaAccount" measure="1" displayFolder="" measureGroup="Shared_DimPagaAccount" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Shared_Organization]" caption="_Count Shared_Organization" measure="1" displayFolder="" measureGroup="Shared_Organization" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_OrganizationUnitHierarcy]" caption="_Count Shared_OrganizationUnitHierarcy" measure="1" displayFolder="" measureGroup="Shared_OrganizationUnitHierarcy" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimCompletedDate]" caption="_Count Shared_DimCompletedDate" measure="1" displayFolder="" measureGroup="Shared_DimCompletedDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimEffectiveDate]" caption="_Count Shared_DimEffectiveDate" measure="1" displayFolder="" measureGroup="Shared_DimEffectiveDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimIntegrationTxDate]" caption="_Count Shared_DimIntegrationTxDate" measure="1" displayFolder="" measureGroup="Shared_DimIntegrationTxDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimStartedDate]" caption="_Count Shared_DimStartedDate" measure="1" displayFolder="" measureGroup="Shared_DimStartedDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimTransactionDate]" caption="_Count Shared_DimTransactionDate" measure="1" displayFolder="" measureGroup="Shared_DimTransactionDate" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_ChartOfAccounts]" caption="_Count Finance_ChartOfAccounts" measure="1" displayFolder="" measureGroup="Finance_ChartOfAccounts" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_GLCodeHierarchy]" caption="_Count Finance_GLCodeHierarchy" measure="1" displayFolder="" measureGroup="Finance_GLCodeHierarchy" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count DatePeriods]" caption="_Count DatePeriods" measure="1" displayFolder="" measureGroup="DatePeriods" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count Shared_OrganizationUnitHierarchy]" caption="_Count Shared_OrganizationUnitHierarchy" measure="1" displayFolder="" measureGroup="Shared_OrganizationUnitHierarchy" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count DatePeriodSelector]" caption="_Count DatePeriodSelector" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count DimDate]" caption="_Count DimDate" measure="1" displayFolder="" measureGroup="DimDate" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimEffectiveDate]" caption="_Count Shared_DimEffectiveDate" measure="1" displayFolder="" measureGroup="Shared_DimEffectiveDate" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimTransactionDate]" caption="_Count Shared_DimTransactionDate" measure="1" displayFolder="" measureGroup="Shared_DimTransactionDate" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
   </cacheHierarchies>
   <kpis count="0"/>
@@ -1186,6 +1396,9 @@
     <dimension name="Classification_DimProcessChannel" uniqueName="[Classification_DimProcessChannel]" caption="Classification_DimProcessChannel"/>
     <dimension name="Classification_DimProcessStatus" uniqueName="[Classification_DimProcessStatus]" caption="Classification_DimProcessStatus"/>
     <dimension name="Classification_DimProcessType" uniqueName="[Classification_DimProcessType]" caption="Classification_DimProcessType"/>
+    <dimension name="DatePeriods" uniqueName="[DatePeriods]" caption="DatePeriods"/>
+    <dimension name="DatePeriodSelector" uniqueName="[DatePeriodSelector]" caption="DatePeriodSelector"/>
+    <dimension name="DimDate" uniqueName="[DimDate]" caption="DimDate"/>
     <dimension name="Finance_ChartOfAccounts" uniqueName="[Finance_ChartOfAccounts]" caption="Finance_ChartOfAccounts"/>
     <dimension name="Finance_DimFinancialAccount" uniqueName="[Finance_DimFinancialAccount]" caption="Finance_DimFinancialAccount"/>
     <dimension name="Finance_FactFinancialTransaction" uniqueName="[Finance_FactFinancialTransaction]" caption="Finance_FactFinancialTransaction"/>
@@ -1194,14 +1407,11 @@
     <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
     <dimension name="Shared_DimApprovingUser" uniqueName="[Shared_DimApprovingUser]" caption="Shared_DimApprovingUser"/>
     <dimension name="Shared_DimCancellingUser" uniqueName="[Shared_DimCancellingUser]" caption="Shared_DimCancellingUser"/>
-    <dimension name="Shared_DimCompletedDate" uniqueName="[Shared_DimCompletedDate]" caption="Shared_DimCompletedDate"/>
     <dimension name="Shared_DimEffectiveDate" uniqueName="[Shared_DimEffectiveDate]" caption="Shared_DimEffectiveDate"/>
     <dimension name="Shared_DimForUser" uniqueName="[Shared_DimForUser]" caption="Shared_DimForUser"/>
     <dimension name="Shared_DimInitiatingUser" uniqueName="[Shared_DimInitiatingUser]" caption="Shared_DimInitiatingUser"/>
-    <dimension name="Shared_DimIntegrationTxDate" uniqueName="[Shared_DimIntegrationTxDate]" caption="Shared_DimIntegrationTxDate"/>
     <dimension name="Shared_DimPagaAccount" uniqueName="[Shared_DimPagaAccount]" caption="Shared_DimPagaAccount"/>
     <dimension name="Shared_DimRole" uniqueName="[Shared_DimRole]" caption="Shared_DimRole"/>
-    <dimension name="Shared_DimStartedDate" uniqueName="[Shared_DimStartedDate]" caption="Shared_DimStartedDate"/>
     <dimension name="Shared_DimToUser" uniqueName="[Shared_DimToUser]" caption="Shared_DimToUser"/>
     <dimension name="Shared_DimTransactionDate" uniqueName="[Shared_DimTransactionDate]" caption="Shared_DimTransactionDate"/>
     <dimension name="Shared_DimUser" uniqueName="[Shared_DimUser]" caption="Shared_DimUser"/>
@@ -1209,7 +1419,7 @@
     <dimension name="Shared_FactIntegrationTransaction" uniqueName="[Shared_FactIntegrationTransaction]" caption="Shared_FactIntegrationTransaction"/>
     <dimension name="Shared_FactProcessEvent" uniqueName="[Shared_FactProcessEvent]" caption="Shared_FactProcessEvent"/>
     <dimension name="Shared_Organization" uniqueName="[Shared_Organization]" caption="Shared_Organization"/>
-    <dimension name="Shared_OrganizationUnitHierarcy" uniqueName="[Shared_OrganizationUnitHierarcy]" caption="Shared_OrganizationUnitHierarcy"/>
+    <dimension name="Shared_OrganizationUnitHierarchy" uniqueName="[Shared_OrganizationUnitHierarchy]" caption="Shared_OrganizationUnitHierarchy"/>
   </dimensions>
   <measureGroups count="32">
     <measureGroup name="Classification_DimAgentCommissionType" caption="Classification_DimAgentCommissionType"/>
@@ -1221,6 +1431,9 @@
     <measureGroup name="Classification_DimProcessChannel" caption="Classification_DimProcessChannel"/>
     <measureGroup name="Classification_DimProcessStatus" caption="Classification_DimProcessStatus"/>
     <measureGroup name="Classification_DimProcessType" caption="Classification_DimProcessType"/>
+    <measureGroup name="DatePeriods" caption="DatePeriods"/>
+    <measureGroup name="DatePeriodSelector" caption="DatePeriodSelector"/>
+    <measureGroup name="DimDate" caption="DimDate"/>
     <measureGroup name="Finance_ChartOfAccounts" caption="Finance_ChartOfAccounts"/>
     <measureGroup name="Finance_DimFinancialAccount" caption="Finance_DimFinancialAccount"/>
     <measureGroup name="Finance_FactFinancialTransaction" caption="Finance_FactFinancialTransaction"/>
@@ -1228,14 +1441,11 @@
     <measureGroup name="Finance_GLCodeHierarchy" caption="Finance_GLCodeHierarchy"/>
     <measureGroup name="Shared_DimApprovingUser" caption="Shared_DimApprovingUser"/>
     <measureGroup name="Shared_DimCancellingUser" caption="Shared_DimCancellingUser"/>
-    <measureGroup name="Shared_DimCompletedDate" caption="Shared_DimCompletedDate"/>
     <measureGroup name="Shared_DimEffectiveDate" caption="Shared_DimEffectiveDate"/>
     <measureGroup name="Shared_DimForUser" caption="Shared_DimForUser"/>
     <measureGroup name="Shared_DimInitiatingUser" caption="Shared_DimInitiatingUser"/>
-    <measureGroup name="Shared_DimIntegrationTxDate" caption="Shared_DimIntegrationTxDate"/>
     <measureGroup name="Shared_DimPagaAccount" caption="Shared_DimPagaAccount"/>
     <measureGroup name="Shared_DimRole" caption="Shared_DimRole"/>
-    <measureGroup name="Shared_DimStartedDate" caption="Shared_DimStartedDate"/>
     <measureGroup name="Shared_DimToUser" caption="Shared_DimToUser"/>
     <measureGroup name="Shared_DimTransactionDate" caption="Shared_DimTransactionDate"/>
     <measureGroup name="Shared_DimUser" caption="Shared_DimUser"/>
@@ -1243,9 +1453,9 @@
     <measureGroup name="Shared_FactIntegrationTransaction" caption="Shared_FactIntegrationTransaction"/>
     <measureGroup name="Shared_FactProcessEvent" caption="Shared_FactProcessEvent"/>
     <measureGroup name="Shared_Organization" caption="Shared_Organization"/>
-    <measureGroup name="Shared_OrganizationUnitHierarcy" caption="Shared_OrganizationUnitHierarcy"/>
+    <measureGroup name="Shared_OrganizationUnitHierarchy" caption="Shared_OrganizationUnitHierarchy"/>
   </measureGroups>
-  <maps count="77">
+  <maps count="74">
     <map measureGroup="0" dimension="0"/>
     <map measureGroup="1" dimension="1"/>
     <map measureGroup="2" dimension="2"/>
@@ -1256,50 +1466,49 @@
     <map measureGroup="7" dimension="7"/>
     <map measureGroup="8" dimension="8"/>
     <map measureGroup="9" dimension="9"/>
-    <map measureGroup="10" dimension="5"/>
     <map measureGroup="10" dimension="10"/>
-    <map measureGroup="10" dimension="22"/>
-    <map measureGroup="11" dimension="2"/>
     <map measureGroup="11" dimension="11"/>
-    <map measureGroup="11" dimension="18"/>
-    <map measureGroup="11" dimension="23"/>
-    <map measureGroup="11" dimension="26"/>
-    <map measureGroup="11" dimension="27"/>
-    <map measureGroup="12" dimension="2"/>
-    <map measureGroup="12" dimension="5"/>
-    <map measureGroup="12" dimension="9"/>
-    <map measureGroup="12" dimension="10"/>
-    <map measureGroup="12" dimension="11"/>
     <map measureGroup="12" dimension="12"/>
-    <map measureGroup="12" dimension="13"/>
-    <map measureGroup="12" dimension="18"/>
-    <map measureGroup="12" dimension="22"/>
-    <map measureGroup="12" dimension="23"/>
-    <map measureGroup="12" dimension="26"/>
-    <map measureGroup="12" dimension="27"/>
-    <map measureGroup="13" dimension="9"/>
+    <map measureGroup="13" dimension="5"/>
     <map measureGroup="13" dimension="13"/>
-    <map measureGroup="14" dimension="15"/>
+    <map measureGroup="13" dimension="23"/>
+    <map measureGroup="14" dimension="2"/>
+    <map measureGroup="14" dimension="14"/>
+    <map measureGroup="14" dimension="20"/>
+    <map measureGroup="14" dimension="24"/>
+    <map measureGroup="14" dimension="27"/>
+    <map measureGroup="15" dimension="2"/>
+    <map measureGroup="15" dimension="5"/>
+    <map measureGroup="15" dimension="10"/>
+    <map measureGroup="15" dimension="12"/>
+    <map measureGroup="15" dimension="13"/>
+    <map measureGroup="15" dimension="14"/>
+    <map measureGroup="15" dimension="15"/>
     <map measureGroup="15" dimension="16"/>
-    <map measureGroup="16" dimension="17"/>
+    <map measureGroup="15" dimension="20"/>
+    <map measureGroup="15" dimension="23"/>
+    <map measureGroup="15" dimension="24"/>
+    <map measureGroup="15" dimension="26"/>
+    <map measureGroup="15" dimension="27"/>
+    <map measureGroup="16" dimension="12"/>
+    <map measureGroup="16" dimension="16"/>
     <map measureGroup="17" dimension="18"/>
     <map measureGroup="18" dimension="19"/>
     <map measureGroup="19" dimension="20"/>
     <map measureGroup="20" dimension="21"/>
-    <map measureGroup="21" dimension="5"/>
     <map measureGroup="21" dimension="22"/>
+    <map measureGroup="22" dimension="5"/>
     <map measureGroup="22" dimension="23"/>
     <map measureGroup="23" dimension="24"/>
     <map measureGroup="24" dimension="25"/>
     <map measureGroup="25" dimension="26"/>
-    <map measureGroup="26" dimension="23"/>
+    <map measureGroup="26" dimension="24"/>
     <map measureGroup="26" dimension="27"/>
     <map measureGroup="27" dimension="28"/>
     <map measureGroup="28" dimension="1"/>
     <map measureGroup="28" dimension="3"/>
     <map measureGroup="28" dimension="4"/>
-    <map measureGroup="28" dimension="21"/>
-    <map measureGroup="28" dimension="23"/>
+    <map measureGroup="28" dimension="24"/>
     <map measureGroup="28" dimension="27"/>
     <map measureGroup="28" dimension="29"/>
     <map measureGroup="28" dimension="31"/>
@@ -1307,12 +1516,10 @@
     <map measureGroup="29" dimension="6"/>
     <map measureGroup="29" dimension="7"/>
     <map measureGroup="29" dimension="8"/>
-    <map measureGroup="29" dimension="15"/>
-    <map measureGroup="29" dimension="16"/>
-    <map measureGroup="29" dimension="17"/>
+    <map measureGroup="29" dimension="18"/>
     <map measureGroup="29" dimension="19"/>
-    <map measureGroup="29" dimension="20"/>
-    <map measureGroup="29" dimension="23"/>
+    <map measureGroup="29" dimension="21"/>
+    <map measureGroup="29" dimension="22"/>
     <map measureGroup="29" dimension="24"/>
     <map measureGroup="29" dimension="25"/>
     <map measureGroup="29" dimension="27"/>
@@ -1333,7 +1540,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42055.410697569445" backgroundQuery="1" createdVersion="3" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Christina Leo" refreshedDate="42055.646040509258" backgroundQuery="1" createdVersion="3" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1">
     <extLst>
       <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
@@ -1342,7 +1549,7 @@
     </extLst>
   </cacheSource>
   <cacheFields count="0"/>
-  <cacheHierarchies count="396">
+  <cacheHierarchies count="455">
     <cacheHierarchy uniqueName="[Classification_DimAgentCommissionType].[DimAgentCommissionTypeID]" caption="DimAgentCommissionTypeID" attribute="1" defaultMemberUniqueName="[Classification_DimAgentCommissionType].[DimAgentCommissionTypeID].[All]" allUniqueName="[Classification_DimAgentCommissionType].[DimAgentCommissionTypeID].[All]" dimensionUniqueName="[Classification_DimAgentCommissionType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimAgentCommissionType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Classification_DimAgentCommissionType].[Name].[All]" allUniqueName="[Classification_DimAgentCommissionType].[Name].[All]" dimensionUniqueName="[Classification_DimAgentCommissionType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimAgentCommissionType].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Classification_DimAgentCommissionType].[SourceKey].[All]" allUniqueName="[Classification_DimAgentCommissionType].[SourceKey].[All]" dimensionUniqueName="[Classification_DimAgentCommissionType]" displayFolder="" count="0" unbalanced="0"/>
@@ -1373,6 +1580,66 @@
     <cacheHierarchy uniqueName="[Classification_DimProcessType].[DimProcessTypeID]" caption="DimProcessTypeID" attribute="1" defaultMemberUniqueName="[Classification_DimProcessType].[DimProcessTypeID].[All]" allUniqueName="[Classification_DimProcessType].[DimProcessTypeID].[All]" dimensionUniqueName="[Classification_DimProcessType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimProcessType].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Classification_DimProcessType].[Name].[All]" allUniqueName="[Classification_DimProcessType].[Name].[All]" dimensionUniqueName="[Classification_DimProcessType]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Classification_DimProcessType].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Classification_DimProcessType].[SourceKey].[All]" allUniqueName="[Classification_DimProcessType].[SourceKey].[All]" dimensionUniqueName="[Classification_DimProcessType]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[Aggregate]" caption="Aggregate" attribute="1" defaultMemberUniqueName="[DatePeriods].[Aggregate].[All]" allUniqueName="[DatePeriods].[Aggregate].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[Number]" caption="Number" attribute="1" defaultMemberUniqueName="[DatePeriods].[Number].[All]" allUniqueName="[DatePeriods].[Number].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[OrderNumber]" caption="OrderNumber" attribute="1" defaultMemberUniqueName="[DatePeriods].[OrderNumber].[All]" allUniqueName="[DatePeriods].[OrderNumber].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[Period]" caption="Period" attribute="1" defaultMemberUniqueName="[DatePeriods].[Period].[All]" allUniqueName="[DatePeriods].[Period].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[PeriodName]" caption="PeriodName" attribute="1" defaultMemberUniqueName="[DatePeriods].[PeriodName].[All]" allUniqueName="[DatePeriods].[PeriodName].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriods].[PeriodType]" caption="PeriodType" attribute="1" defaultMemberUniqueName="[DatePeriods].[PeriodType].[All]" allUniqueName="[DatePeriods].[PeriodType].[All]" dimensionUniqueName="[DatePeriods]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[Date].[All]" allUniqueName="[DatePeriodSelector].[Date].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DateID].[All]" allUniqueName="[DatePeriodSelector].[DateID].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DateSK].[All]" allUniqueName="[DatePeriodSelector].[DateSK].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[Day].[All]" allUniqueName="[DatePeriodSelector].[Day].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DayOfWeek].[All]" allUniqueName="[DatePeriodSelector].[DayOfWeek].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DayOfYear].[All]" allUniqueName="[DatePeriodSelector].[DayOfYear].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DaySuffix].[All]" allUniqueName="[DatePeriodSelector].[DaySuffix].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[DOWInMonth].[All]" allUniqueName="[DatePeriodSelector].[DOWInMonth].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialPeriodAllTime].[All]" allUniqueName="[DatePeriodSelector].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialPeriodName].[All]" allUniqueName="[DatePeriodSelector].[FinancialPeriodName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialPeriodNumber].[All]" allUniqueName="[DatePeriodSelector].[FinancialPeriodNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialYearName].[All]" allUniqueName="[DatePeriodSelector].[FinancialYearName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[FinancialYearNumber].[All]" allUniqueName="[DatePeriodSelector].[FinancialYearNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[HolidayText].[All]" allUniqueName="[DatePeriodSelector].[HolidayText].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[IsPublicHoliday].[All]" allUniqueName="[DatePeriodSelector].[IsPublicHoliday].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[MonthAllTime].[All]" allUniqueName="[DatePeriodSelector].[MonthAllTime].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[MonthName].[All]" allUniqueName="[DatePeriodSelector].[MonthName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[MonthNumber].[All]" allUniqueName="[DatePeriodSelector].[MonthNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[Quarter].[All]" allUniqueName="[DatePeriodSelector].[Quarter].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[QuarterAllTime].[All]" allUniqueName="[DatePeriodSelector].[QuarterAllTime].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[QuarterName].[All]" allUniqueName="[DatePeriodSelector].[QuarterName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[StandardDate].[All]" allUniqueName="[DatePeriodSelector].[StandardDate].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[USDayOfWeek].[All]" allUniqueName="[DatePeriodSelector].[USDayOfWeek].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[WeekOfMonth].[All]" allUniqueName="[DatePeriodSelector].[WeekOfMonth].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[WeekOfYear].[All]" allUniqueName="[DatePeriodSelector].[WeekOfYear].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[YearName].[All]" allUniqueName="[DatePeriodSelector].[YearName].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DatePeriodSelector].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[DatePeriodSelector].[YearNumber].[All]" allUniqueName="[DatePeriodSelector].[YearNumber].[All]" dimensionUniqueName="[DatePeriodSelector]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[DimDate].[Date].[All]" allUniqueName="[DimDate].[Date].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[DimDate].[DateID].[All]" allUniqueName="[DimDate].[DateID].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[DimDate].[DateSK].[All]" allUniqueName="[DimDate].[DateSK].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[DimDate].[Day].[All]" allUniqueName="[DimDate].[Day].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[DimDate].[DayOfWeek].[All]" allUniqueName="[DimDate].[DayOfWeek].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[DimDate].[DayOfYear].[All]" allUniqueName="[DimDate].[DayOfYear].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[DimDate].[DaySuffix].[All]" allUniqueName="[DimDate].[DaySuffix].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[DimDate].[DOWInMonth].[All]" allUniqueName="[DimDate].[DOWInMonth].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialPeriodAllTime].[All]" allUniqueName="[DimDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialPeriodName].[All]" allUniqueName="[DimDate].[FinancialPeriodName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialPeriodNumber].[All]" allUniqueName="[DimDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialYearName].[All]" allUniqueName="[DimDate].[FinancialYearName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[DimDate].[FinancialYearNumber].[All]" allUniqueName="[DimDate].[FinancialYearNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[DimDate].[HolidayText].[All]" allUniqueName="[DimDate].[HolidayText].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[DimDate].[IsPublicHoliday].[All]" allUniqueName="[DimDate].[IsPublicHoliday].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[DimDate].[MonthAllTime].[All]" allUniqueName="[DimDate].[MonthAllTime].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[DimDate].[MonthName].[All]" allUniqueName="[DimDate].[MonthName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[DimDate].[MonthNumber].[All]" allUniqueName="[DimDate].[MonthNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[DimDate].[Quarter].[All]" allUniqueName="[DimDate].[Quarter].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[DimDate].[QuarterAllTime].[All]" allUniqueName="[DimDate].[QuarterAllTime].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[DimDate].[QuarterName].[All]" allUniqueName="[DimDate].[QuarterName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[DimDate].[StandardDate].[All]" allUniqueName="[DimDate].[StandardDate].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[DimDate].[USDayOfWeek].[All]" allUniqueName="[DimDate].[USDayOfWeek].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[DimDate].[WeekOfMonth].[All]" allUniqueName="[DimDate].[WeekOfMonth].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[DimDate].[WeekOfYear].[All]" allUniqueName="[DimDate].[WeekOfYear].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[DimDate].[YearName].[All]" allUniqueName="[DimDate].[YearName].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[DimDate].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[DimDate].[YearNumber].[All]" allUniqueName="[DimDate].[YearNumber].[All]" dimensionUniqueName="[DimDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_ChartOfAccounts].[COA_CodeRange]" caption="COA_CodeRange" attribute="1" defaultMemberUniqueName="[Finance_ChartOfAccounts].[COA_CodeRange].[All]" allUniqueName="[Finance_ChartOfAccounts].[COA_CodeRange].[All]" dimensionUniqueName="[Finance_ChartOfAccounts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_ChartOfAccounts].[COA_Name]" caption="COA_Name" attribute="1" defaultMemberUniqueName="[Finance_ChartOfAccounts].[COA_Name].[All]" allUniqueName="[Finance_ChartOfAccounts].[COA_Name].[All]" dimensionUniqueName="[Finance_ChartOfAccounts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_ChartOfAccounts].[DimChartOfAccountsID]" caption="DimChartOfAccountsID" attribute="1" defaultMemberUniqueName="[Finance_ChartOfAccounts].[DimChartOfAccountsID].[All]" allUniqueName="[Finance_ChartOfAccounts].[DimChartOfAccountsID].[All]" dimensionUniqueName="[Finance_ChartOfAccounts]" displayFolder="" count="0" unbalanced="0"/>
@@ -1380,9 +1647,9 @@
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimBankAccountID]" caption="DimBankAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimBankAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimBankAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimCurrencyID]" caption="DimCurrencyID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimCurrencyID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimCurrencyID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountID]" caption="DimFinancialAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountTypeID]" caption="DimFinancialAccountTypeID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountTypeID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimFinancialAccountTypeID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimFinancialHoldingAccountID]" caption="DimFinancialHoldingAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimFinancialHoldingAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimFinancialHoldingAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[DimPagaAccountID].[All]" allUniqueName="[Finance_DimFinancialAccount].[DimPagaAccountID].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[FinancialAccountType]" caption="FinancialAccountType" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[FinancialAccountType].[All]" allUniqueName="[Finance_DimFinancialAccount].[FinancialAccountType].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[Name].[All]" allUniqueName="[Finance_DimFinancialAccount].[Name].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[OpeningBalance]" caption="OpeningBalance" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[OpeningBalance].[All]" allUniqueName="[Finance_DimFinancialAccount].[OpeningBalance].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_DimFinancialAccount].[RestrictedBalance]" caption="RestrictedBalance" attribute="1" defaultMemberUniqueName="[Finance_DimFinancialAccount].[RestrictedBalance].[All]" allUniqueName="[Finance_DimFinancialAccount].[RestrictedBalance].[All]" dimensionUniqueName="[Finance_DimFinancialAccount]" displayFolder="" count="0" unbalanced="0"/>
@@ -1412,6 +1679,7 @@
     <cacheHierarchy uniqueName="[Finance_FactFinancialTransaction].[ShortCode]" caption="ShortCode" attribute="1" defaultMemberUniqueName="[Finance_FactFinancialTransaction].[ShortCode].[All]" allUniqueName="[Finance_FactFinancialTransaction].[ShortCode].[All]" dimensionUniqueName="[Finance_FactFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactFinancialTransaction].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Finance_FactFinancialTransaction].[SourceKey].[All]" allUniqueName="[Finance_FactFinancialTransaction].[SourceKey].[All]" dimensionUniqueName="[Finance_FactFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactFinancialTransaction].[TextDescription]" caption="TextDescription" attribute="1" defaultMemberUniqueName="[Finance_FactFinancialTransaction].[TextDescription].[All]" allUniqueName="[Finance_FactFinancialTransaction].[TextDescription].[All]" dimensionUniqueName="[Finance_FactFinancialTransaction]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[Balance]" caption="Balance" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[Balance].[All]" allUniqueName="[Finance_FactGLTransaction].[Balance].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[CreditAmount]" caption="CreditAmount" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[CreditAmount].[All]" allUniqueName="[Finance_FactGLTransaction].[CreditAmount].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[DebitAmount]" caption="DebitAmount" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[DebitAmount].[All]" allUniqueName="[Finance_FactGLTransaction].[DebitAmount].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Finance_FactGLTransaction].[DimFinancialAccountID]" caption="DimFinancialAccountID" attribute="1" defaultMemberUniqueName="[Finance_FactGLTransaction].[DimFinancialAccountID].[All]" allUniqueName="[Finance_FactGLTransaction].[DimFinancialAccountID].[All]" dimensionUniqueName="[Finance_FactGLTransaction]" displayFolder="" count="0" unbalanced="0"/>
@@ -1457,32 +1725,33 @@
     <cacheHierarchy uniqueName="[Shared_DimCancellingUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Shared_DimCancellingUser].[Name].[All]" allUniqueName="[Shared_DimCancellingUser].[Name].[All]" dimensionUniqueName="[Shared_DimCancellingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimCancellingUser].[PhoneNumber]" caption="PhoneNumber" attribute="1" defaultMemberUniqueName="[Shared_DimCancellingUser].[PhoneNumber].[All]" allUniqueName="[Shared_DimCancellingUser].[PhoneNumber].[All]" dimensionUniqueName="[Shared_DimCancellingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimCancellingUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimCancellingUser].[SourceKey].[All]" allUniqueName="[Shared_DimCancellingUser].[SourceKey].[All]" dimensionUniqueName="[Shared_DimCancellingUser]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DayName].[All]" allUniqueName="[Shared_DimCompletedDate].[DayName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimCompletedDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DayOfYear].[All]" allUniqueName="[Shared_DimCompletedDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[DimCompletedDateID]" caption="DimCompletedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[DimCompletedDateID].[All]" allUniqueName="[Shared_DimCompletedDate].[DimCompletedDateID].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[FullDate].[All]" allUniqueName="[Shared_DimCompletedDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[MMYYYY].[All]" allUniqueName="[Shared_DimCompletedDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[Month].[All]" allUniqueName="[Shared_DimCompletedDate].[Month].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[MonthName].[All]" allUniqueName="[Shared_DimCompletedDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[MonthYear].[All]" allUniqueName="[Shared_DimCompletedDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[Quarter].[All]" allUniqueName="[Shared_DimCompletedDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[QuarterName].[All]" allUniqueName="[Shared_DimCompletedDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[Year].[All]" allUniqueName="[Shared_DimCompletedDate].[Year].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimCompletedDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimCompletedDate].[YearName].[All]" allUniqueName="[Shared_DimCompletedDate].[YearName].[All]" dimensionUniqueName="[Shared_DimCompletedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayName].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Date].[All]" allUniqueName="[Shared_DimEffectiveDate].[Date].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DateID].[All]" allUniqueName="[Shared_DimEffectiveDate].[DateID].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DateSK].[All]" allUniqueName="[Shared_DimEffectiveDate].[DateSK].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Day].[All]" allUniqueName="[Shared_DimEffectiveDate].[Day].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayOfWeek].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayOfWeek].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DayOfYear].[All]" allUniqueName="[Shared_DimEffectiveDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DimEffectiveDateID]" caption="DimEffectiveDateID" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DimEffectiveDateID].[All]" allUniqueName="[Shared_DimEffectiveDate].[DimEffectiveDateID].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FullDate].[All]" allUniqueName="[Shared_DimEffectiveDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MMYYYY].[All]" allUniqueName="[Shared_DimEffectiveDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Month].[All]" allUniqueName="[Shared_DimEffectiveDate].[Month].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DaySuffix].[All]" allUniqueName="[Shared_DimEffectiveDate].[DaySuffix].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[DOWInMonth].[All]" allUniqueName="[Shared_DimEffectiveDate].[DOWInMonth].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodAllTime].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodName].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialYearName].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialYearName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[FinancialYearNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[FinancialYearNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[HolidayText].[All]" allUniqueName="[Shared_DimEffectiveDate].[HolidayText].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[IsPublicHoliday].[All]" allUniqueName="[Shared_DimEffectiveDate].[IsPublicHoliday].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthAllTime].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthAllTime].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthName].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthYear].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[MonthNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[MonthNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Quarter].[All]" allUniqueName="[Shared_DimEffectiveDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[QuarterAllTime].[All]" allUniqueName="[Shared_DimEffectiveDate].[QuarterAllTime].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[QuarterName].[All]" allUniqueName="[Shared_DimEffectiveDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[Year].[All]" allUniqueName="[Shared_DimEffectiveDate].[Year].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[StandardDate].[All]" allUniqueName="[Shared_DimEffectiveDate].[StandardDate].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[USDayOfWeek].[All]" allUniqueName="[Shared_DimEffectiveDate].[USDayOfWeek].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[WeekOfMonth].[All]" allUniqueName="[Shared_DimEffectiveDate].[WeekOfMonth].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[WeekOfYear].[All]" allUniqueName="[Shared_DimEffectiveDate].[WeekOfYear].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[YearName].[All]" allUniqueName="[Shared_DimEffectiveDate].[YearName].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimEffectiveDate].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimEffectiveDate].[YearNumber].[All]" allUniqueName="[Shared_DimEffectiveDate].[YearNumber].[All]" dimensionUniqueName="[Shared_DimEffectiveDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimForUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimForUser].[DimCreatedDateID].[All]" allUniqueName="[Shared_DimForUser].[DimCreatedDateID].[All]" dimensionUniqueName="[Shared_DimForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimForUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[Shared_DimForUser].[DimDateOfBirthID].[All]" allUniqueName="[Shared_DimForUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[Shared_DimForUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimForUser].[DimForUserID]" caption="DimForUserID" attribute="1" defaultMemberUniqueName="[Shared_DimForUser].[DimForUserID].[All]" allUniqueName="[Shared_DimForUser].[DimForUserID].[All]" dimensionUniqueName="[Shared_DimForUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -1509,19 +1778,6 @@
     <cacheHierarchy uniqueName="[Shared_DimInitiatingUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Shared_DimInitiatingUser].[Name].[All]" allUniqueName="[Shared_DimInitiatingUser].[Name].[All]" dimensionUniqueName="[Shared_DimInitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimInitiatingUser].[PhoneNumber]" caption="PhoneNumber" attribute="1" defaultMemberUniqueName="[Shared_DimInitiatingUser].[PhoneNumber].[All]" allUniqueName="[Shared_DimInitiatingUser].[PhoneNumber].[All]" dimensionUniqueName="[Shared_DimInitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimInitiatingUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimInitiatingUser].[SourceKey].[All]" allUniqueName="[Shared_DimInitiatingUser].[SourceKey].[All]" dimensionUniqueName="[Shared_DimInitiatingUser]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DayName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DayName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DayOfYear].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[DimIntegrationTxDateID]" caption="DimIntegrationTxDateID" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[DimIntegrationTxDateID].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[DimIntegrationTxDateID].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[FullDate].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[MMYYYY].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[Month].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[Month].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[MonthName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[MonthYear].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[Quarter].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[QuarterName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[Year].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[Year].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimIntegrationTxDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimIntegrationTxDate].[YearName].[All]" allUniqueName="[Shared_DimIntegrationTxDate].[YearName].[All]" dimensionUniqueName="[Shared_DimIntegrationTxDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimPagaAccount].[BankingStatus]" caption="BankingStatus" attribute="1" defaultMemberUniqueName="[Shared_DimPagaAccount].[BankingStatus].[All]" allUniqueName="[Shared_DimPagaAccount].[BankingStatus].[All]" dimensionUniqueName="[Shared_DimPagaAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimPagaAccount].[CreatedDateID]" caption="CreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimPagaAccount].[CreatedDateID].[All]" allUniqueName="[Shared_DimPagaAccount].[CreatedDateID].[All]" dimensionUniqueName="[Shared_DimPagaAccount]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimPagaAccount].[DimPagaAccountID]" caption="DimPagaAccountID" attribute="1" defaultMemberUniqueName="[Shared_DimPagaAccount].[DimPagaAccountID].[All]" allUniqueName="[Shared_DimPagaAccount].[DimPagaAccountID].[All]" dimensionUniqueName="[Shared_DimPagaAccount]" displayFolder="" count="0" unbalanced="0"/>
@@ -1551,19 +1807,6 @@
     <cacheHierarchy uniqueName="[Shared_DimRole].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimRole].[SourceKey].[All]" allUniqueName="[Shared_DimRole].[SourceKey].[All]" dimensionUniqueName="[Shared_DimRole]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimRole].[SystemDescription]" caption="SystemDescription" attribute="1" defaultMemberUniqueName="[Shared_DimRole].[SystemDescription].[All]" allUniqueName="[Shared_DimRole].[SystemDescription].[All]" dimensionUniqueName="[Shared_DimRole]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimRole].[TextDesciption]" caption="TextDesciption" attribute="1" defaultMemberUniqueName="[Shared_DimRole].[TextDesciption].[All]" allUniqueName="[Shared_DimRole].[TextDesciption].[All]" dimensionUniqueName="[Shared_DimRole]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DayName].[All]" allUniqueName="[Shared_DimStartedDate].[DayName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimStartedDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DayOfYear].[All]" allUniqueName="[Shared_DimStartedDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[DimStartedDateID]" caption="DimStartedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[DimStartedDateID].[All]" allUniqueName="[Shared_DimStartedDate].[DimStartedDateID].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[FullDate].[All]" allUniqueName="[Shared_DimStartedDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[MMYYYY].[All]" allUniqueName="[Shared_DimStartedDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[Month].[All]" allUniqueName="[Shared_DimStartedDate].[Month].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[MonthName].[All]" allUniqueName="[Shared_DimStartedDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[MonthYear].[All]" allUniqueName="[Shared_DimStartedDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[Quarter].[All]" allUniqueName="[Shared_DimStartedDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[QuarterName].[All]" allUniqueName="[Shared_DimStartedDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[Year].[All]" allUniqueName="[Shared_DimStartedDate].[Year].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimStartedDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimStartedDate].[YearName].[All]" allUniqueName="[Shared_DimStartedDate].[YearName].[All]" dimensionUniqueName="[Shared_DimStartedDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[DimCreatedDateID].[All]" allUniqueName="[Shared_DimToUser].[DimCreatedDateID].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[DimDateOfBirthID].[All]" allUniqueName="[Shared_DimToUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[DimPrimaryRoleID]" caption="DimPrimaryRoleID" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[DimPrimaryRoleID].[All]" allUniqueName="[Shared_DimToUser].[DimPrimaryRoleID].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -1577,19 +1820,33 @@
     <cacheHierarchy uniqueName="[Shared_DimToUser].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[Name].[All]" allUniqueName="[Shared_DimToUser].[Name].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[PhoneNumber]" caption="PhoneNumber" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[PhoneNumber].[All]" allUniqueName="[Shared_DimToUser].[PhoneNumber].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimToUser].[SourceKey]" caption="SourceKey" attribute="1" defaultMemberUniqueName="[Shared_DimToUser].[SourceKey].[All]" allUniqueName="[Shared_DimToUser].[SourceKey].[All]" dimensionUniqueName="[Shared_DimToUser]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayName]" caption="DayName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayName].[All]" allUniqueName="[Shared_DimTransactionDate].[DayName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayOfMonth]" caption="DayOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayOfMonth].[All]" allUniqueName="[Shared_DimTransactionDate].[DayOfMonth].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DimTransactionDateID]" caption="DimTransactionDateID" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DimTransactionDateID].[All]" allUniqueName="[Shared_DimTransactionDate].[DimTransactionDateID].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FullDate]" caption="FullDate" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FullDate].[All]" allUniqueName="[Shared_DimTransactionDate].[FullDate].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Hierarchy1]" caption="Hierarchy1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Hierarchy1].[All]" allUniqueName="[Shared_DimTransactionDate].[Hierarchy1].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MMYYYY]" caption="MMYYYY" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MMYYYY].[All]" allUniqueName="[Shared_DimTransactionDate].[MMYYYY].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Month].[All]" allUniqueName="[Shared_DimTransactionDate].[Month].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Date]" caption="Date" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Date].[All]" allUniqueName="[Shared_DimTransactionDate].[Date].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DateID]" caption="DateID" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DateID].[All]" allUniqueName="[Shared_DimTransactionDate].[DateID].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DateSK]" caption="DateSK" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DateSK].[All]" allUniqueName="[Shared_DimTransactionDate].[DateSK].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Day].[All]" allUniqueName="[Shared_DimTransactionDate].[Day].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayOfWeek]" caption="DayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayOfWeek].[All]" allUniqueName="[Shared_DimTransactionDate].[DayOfWeek].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DayOfYear]" caption="DayOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DayOfYear].[All]" allUniqueName="[Shared_DimTransactionDate].[DayOfYear].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DaySuffix]" caption="DaySuffix" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DaySuffix].[All]" allUniqueName="[Shared_DimTransactionDate].[DaySuffix].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[DOWInMonth]" caption="DOWInMonth" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[DOWInMonth].[All]" allUniqueName="[Shared_DimTransactionDate].[DOWInMonth].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialPeriodAllTime]" caption="FinancialPeriodAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialPeriodAllTime].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialPeriodAllTime].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialPeriodName]" caption="FinancialPeriodName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialPeriodName].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialPeriodName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialPeriodNumber]" caption="FinancialPeriodNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialPeriodNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialPeriodNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialYearName]" caption="FinancialYearName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialYearName].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialYearName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[FinancialYearNumber]" caption="FinancialYearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[FinancialYearNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[FinancialYearNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[HolidayText]" caption="HolidayText" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[HolidayText].[All]" allUniqueName="[Shared_DimTransactionDate].[HolidayText].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[IsPublicHoliday]" caption="IsPublicHoliday" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[IsPublicHoliday].[All]" allUniqueName="[Shared_DimTransactionDate].[IsPublicHoliday].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthAllTime]" caption="MonthAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthAllTime].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthAllTime].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthName]" caption="MonthName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthName].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthYear]" caption="MonthYear" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthYear].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthYear].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[MonthNumber]" caption="MonthNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[MonthNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[MonthNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Quarter].[All]" allUniqueName="[Shared_DimTransactionDate].[Quarter].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[QuarterAllTime]" caption="QuarterAllTime" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[QuarterAllTime].[All]" allUniqueName="[Shared_DimTransactionDate].[QuarterAllTime].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[QuarterName]" caption="QuarterName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[QuarterName].[All]" allUniqueName="[Shared_DimTransactionDate].[QuarterName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[Year].[All]" allUniqueName="[Shared_DimTransactionDate].[Year].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[StandardDate]" caption="StandardDate" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[StandardDate].[All]" allUniqueName="[Shared_DimTransactionDate].[StandardDate].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[USDayOfWeek]" caption="USDayOfWeek" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[USDayOfWeek].[All]" allUniqueName="[Shared_DimTransactionDate].[USDayOfWeek].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[WeekOfMonth]" caption="WeekOfMonth" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[WeekOfMonth].[All]" allUniqueName="[Shared_DimTransactionDate].[WeekOfMonth].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[WeekOfYear]" caption="WeekOfYear" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[WeekOfYear].[All]" allUniqueName="[Shared_DimTransactionDate].[WeekOfYear].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[YearName]" caption="YearName" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[YearName].[All]" allUniqueName="[Shared_DimTransactionDate].[YearName].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_DimTransactionDate].[YearNumber]" caption="YearNumber" attribute="1" defaultMemberUniqueName="[Shared_DimTransactionDate].[YearNumber].[All]" allUniqueName="[Shared_DimTransactionDate].[YearNumber].[All]" dimensionUniqueName="[Shared_DimTransactionDate]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimUser].[DimCreatedDateID]" caption="DimCreatedDateID" attribute="1" defaultMemberUniqueName="[Shared_DimUser].[DimCreatedDateID].[All]" allUniqueName="[Shared_DimUser].[DimCreatedDateID].[All]" dimensionUniqueName="[Shared_DimUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimUser].[DimDateOfBirthID]" caption="DimDateOfBirthID" attribute="1" defaultMemberUniqueName="[Shared_DimUser].[DimDateOfBirthID].[All]" allUniqueName="[Shared_DimUser].[DimDateOfBirthID].[All]" dimensionUniqueName="[Shared_DimUser]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_DimUser].[DimPrimaryRoleID]" caption="DimPrimaryRoleID" attribute="1" defaultMemberUniqueName="[Shared_DimUser].[DimPrimaryRoleID].[All]" allUniqueName="[Shared_DimUser].[DimPrimaryRoleID].[All]" dimensionUniqueName="[Shared_DimUser]" displayFolder="" count="0" unbalanced="0"/>
@@ -1684,28 +1941,37 @@
     <cacheHierarchy uniqueName="[Shared_Organization].[TextDesciption]" caption="TextDesciption" attribute="1" defaultMemberUniqueName="[Shared_Organization].[TextDesciption].[All]" allUniqueName="[Shared_Organization].[TextDesciption].[All]" dimensionUniqueName="[Shared_Organization]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_Organization].[VATCertificationNumber]" caption="VATCertificationNumber" attribute="1" defaultMemberUniqueName="[Shared_Organization].[VATCertificationNumber].[All]" allUniqueName="[Shared_Organization].[VATCertificationNumber].[All]" dimensionUniqueName="[Shared_Organization]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Shared_Organization].[WebsiteURL]" caption="WebsiteURL" attribute="1" defaultMemberUniqueName="[Shared_Organization].[WebsiteURL].[All]" allUniqueName="[Shared_Organization].[WebsiteURL].[All]" dimensionUniqueName="[Shared_Organization]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationID]" caption="DimOrganizationID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel1ID]" caption="DimOrganizationUnitLevel1ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel1ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel1ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel2ID]" caption="DimOrganizationUnitLevel2ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel2ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel2ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel3ID]" caption="DimOrganizationUnitLevel3ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel3ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel3ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel4ID]" caption="DimOrganizationUnitLevel4ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel4ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[DimOrganizationUnitLevel4ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1]" caption="OrgLevel1" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_IdentificationNumber]" caption="OrgLevel1_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_UnitType]" caption="OrgLevel1_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel1_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2]" caption="OrgLevel2" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_IdentificationNumber]" caption="OrgLevel2_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_UnitType]" caption="OrgLevel2_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel2_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3]" caption="OrgLevel3" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_IdentificationNumber]" caption="OrgLevel3_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_UnitType]" caption="OrgLevel3_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel3_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4]" caption="OrgLevel4" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_IdentificationNumber]" caption="OrgLevel4_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_UnitType]" caption="OrgLevel4_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarcy].[OrgLevel4_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarcy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationID]" caption="DimOrganizationID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel1ID]" caption="DimOrganizationUnitLevel1ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel1ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel1ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel2ID]" caption="DimOrganizationUnitLevel2ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel2ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel2ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel3ID]" caption="DimOrganizationUnitLevel3ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel3ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel3ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel4ID]" caption="DimOrganizationUnitLevel4ID" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel4ID].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[DimOrganizationUnitLevel4ID].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1]" caption="OrgLevel1" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_IdentificationNumber]" caption="OrgLevel1_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_UnitType]" caption="OrgLevel1_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel1_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2]" caption="OrgLevel2" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_IdentificationNumber]" caption="OrgLevel2_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_UnitType]" caption="OrgLevel2_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel2_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3]" caption="OrgLevel3" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_IdentificationNumber]" caption="OrgLevel3_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_UnitType]" caption="OrgLevel3_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel3_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4]" caption="OrgLevel4" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_IdentificationNumber]" caption="OrgLevel4_IdentificationNumber" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_IdentificationNumber].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_IdentificationNumber].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_UnitType]" caption="OrgLevel4_UnitType" attribute="1" defaultMemberUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_UnitType].[All]" allUniqueName="[Shared_OrganizationUnitHierarchy].[OrgLevel4_UnitType].[All]" dimensionUniqueName="[Shared_OrganizationUnitHierarchy]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[TransactionCount]" caption="TransactionCount" measure="1" displayFolder="" measureGroup="Finance_FactFinancialTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[TransactionAmount]" caption="TransactionAmount" measure="1" displayFolder="" measureGroup="Finance_FactFinancialTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[GLCreditAmount]" caption="GLCreditAmount" measure="1" displayFolder="" measureGroup="Finance_FactGLTransaction" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[GLDebitAmount]" caption="GLDebitAmount" measure="1" displayFolder="" measureGroup="Finance_FactGLTransaction" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[GLBalance]" caption="GLBalance" measure="1" displayFolder="" measureGroup="Finance_FactGLTransaction" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[PeriodValue]" caption="PeriodValue" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[PeriodNumber]" caption="PeriodNumber" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[PeriodAggregate]" caption="PeriodAggregate" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[PeriodTypeVal]" caption="PeriodTypeVal" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[FilterStartDateID]" caption="FilterStartDateID" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[FilterEndDateID]" caption="FilterEndDateID" measure="1" displayFolder="" measureGroup="DatePeriods" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Minimum of MonthNumber]" caption="Minimum of MonthNumber" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Maximum of MonthNumber]" caption="Maximum of MonthNumber" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[MinDate]" caption="MinDate" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[MaxDate]" caption="MaxDate" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_FactFinancialTransaction]" caption="_Count Finance_FactFinancialTransaction" measure="1" displayFolder="" measureGroup="Finance_FactFinancialTransaction" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_FactGLTransaction]" caption="_Count Finance_FactGLTransaction" measure="1" displayFolder="" measureGroup="Finance_FactGLTransaction" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimRole]" caption="_Count Shared_DimRole" measure="1" displayFolder="" measureGroup="Shared_DimRole" count="0" hidden="1"/>
@@ -1730,29 +1996,29 @@
     <cacheHierarchy uniqueName="[Measures].[_Count Classification_DimProcessType]" caption="_Count Classification_DimProcessType" measure="1" displayFolder="" measureGroup="Classification_DimProcessType" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimPagaAccount]" caption="_Count Shared_DimPagaAccount" measure="1" displayFolder="" measureGroup="Shared_DimPagaAccount" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Shared_Organization]" caption="_Count Shared_Organization" measure="1" displayFolder="" measureGroup="Shared_Organization" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_OrganizationUnitHierarcy]" caption="_Count Shared_OrganizationUnitHierarcy" measure="1" displayFolder="" measureGroup="Shared_OrganizationUnitHierarcy" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimCompletedDate]" caption="_Count Shared_DimCompletedDate" measure="1" displayFolder="" measureGroup="Shared_DimCompletedDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimEffectiveDate]" caption="_Count Shared_DimEffectiveDate" measure="1" displayFolder="" measureGroup="Shared_DimEffectiveDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimIntegrationTxDate]" caption="_Count Shared_DimIntegrationTxDate" measure="1" displayFolder="" measureGroup="Shared_DimIntegrationTxDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimStartedDate]" caption="_Count Shared_DimStartedDate" measure="1" displayFolder="" measureGroup="Shared_DimStartedDate" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimTransactionDate]" caption="_Count Shared_DimTransactionDate" measure="1" displayFolder="" measureGroup="Shared_DimTransactionDate" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_ChartOfAccounts]" caption="_Count Finance_ChartOfAccounts" measure="1" displayFolder="" measureGroup="Finance_ChartOfAccounts" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[_Count Finance_GLCodeHierarchy]" caption="_Count Finance_GLCodeHierarchy" measure="1" displayFolder="" measureGroup="Finance_GLCodeHierarchy" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count DatePeriods]" caption="_Count DatePeriods" measure="1" displayFolder="" measureGroup="DatePeriods" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count Shared_OrganizationUnitHierarchy]" caption="_Count Shared_OrganizationUnitHierarchy" measure="1" displayFolder="" measureGroup="Shared_OrganizationUnitHierarchy" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count DatePeriodSelector]" caption="_Count DatePeriodSelector" measure="1" displayFolder="" measureGroup="DatePeriodSelector" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count DimDate]" caption="_Count DimDate" measure="1" displayFolder="" measureGroup="DimDate" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimEffectiveDate]" caption="_Count Shared_DimEffectiveDate" measure="1" displayFolder="" measureGroup="Shared_DimEffectiveDate" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[_Count Shared_DimTransactionDate]" caption="_Count Shared_DimTransactionDate" measure="1" displayFolder="" measureGroup="Shared_DimTransactionDate" count="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
   </cacheHierarchies>
   <kpis count="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition slicerData="1" pivotCacheId="2" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+      <x14:pivotCacheDefinition slicerData="1" pivotCacheId="5" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="D7:K46" firstHeaderRow="0" firstDataRow="1" firstDataCol="5"/>
-  <pivotFields count="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="86" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="D7:J52" firstHeaderRow="0" firstDataRow="1" firstDataCol="5" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="11">
     <pivotField name="FinancialTransactionType" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="116">
         <item x="0"/>
@@ -1875,7 +2141,6 @@
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="4">
         <item x="0"/>
@@ -1910,7 +2175,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" allDrilled="1" outline="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="36">
+      <items count="41">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1947,10 +2212,15 @@
         <item x="33"/>
         <item x="34"/>
         <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" allDrilled="1" outline="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="36">
+      <items count="41">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1987,20 +2257,33 @@
         <item x="33"/>
         <item x="34"/>
         <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
       </items>
     </pivotField>
-    <pivotField allDrilled="1" showAll="0" dataSourceSort="1"/>
-    <pivotField showAll="0" dataSourceSort="1"/>
+    <pivotField axis="axisPage" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="1">
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="1">
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="6">
+    <field x="3"/>
     <field x="4"/>
+    <field x="6"/>
     <field x="5"/>
+    <field x="8"/>
     <field x="7"/>
-    <field x="6"/>
-    <field x="9"/>
-    <field x="8"/>
   </rowFields>
-  <rowItems count="39">
+  <rowItems count="45">
     <i>
       <x/>
     </i>
@@ -2057,17 +2340,17 @@
       <x v="10"/>
       <x v="10"/>
     </i>
+    <i r="4">
+      <x v="11"/>
+      <x v="11"/>
+    </i>
+    <i r="4">
+      <x v="12"/>
+      <x v="12"/>
+    </i>
     <i r="2">
       <x v="2"/>
       <x v="2"/>
-      <x v="11"/>
-      <x v="11"/>
-    </i>
-    <i r="4">
-      <x v="12"/>
-      <x v="12"/>
-    </i>
-    <i r="4">
       <x v="13"/>
       <x v="13"/>
     </i>
@@ -2098,6 +2381,22 @@
     <i r="4">
       <x v="20"/>
       <x v="20"/>
+    </i>
+    <i r="4">
+      <x v="21"/>
+      <x v="21"/>
+    </i>
+    <i r="4">
+      <x v="22"/>
+      <x v="22"/>
+    </i>
+    <i r="4">
+      <x v="23"/>
+      <x v="23"/>
+    </i>
+    <i r="4">
+      <x v="24"/>
+      <x v="24"/>
     </i>
     <i>
       <x v="2"/>
@@ -2106,22 +2405,6 @@
       <x v="2"/>
       <x v="3"/>
       <x v="3"/>
-      <x v="21"/>
-      <x v="21"/>
-    </i>
-    <i r="4">
-      <x v="22"/>
-      <x v="22"/>
-    </i>
-    <i r="4">
-      <x v="23"/>
-      <x v="23"/>
-    </i>
-    <i r="4">
-      <x v="24"/>
-      <x v="24"/>
-    </i>
-    <i r="4">
       <x v="25"/>
       <x v="25"/>
     </i>
@@ -2157,52 +2440,123 @@
       <x v="33"/>
       <x v="33"/>
     </i>
+    <i r="4">
+      <x v="34"/>
+      <x v="34"/>
+    </i>
+    <i r="4">
+      <x v="35"/>
+      <x v="35"/>
+    </i>
+    <i r="4">
+      <x v="36"/>
+      <x v="36"/>
+    </i>
+    <i r="4">
+      <x v="37"/>
+      <x v="37"/>
+    </i>
     <i r="2">
       <x v="4"/>
       <x v="4"/>
-      <x v="34"/>
-      <x v="34"/>
+      <x v="38"/>
+      <x v="38"/>
     </i>
     <i r="4">
-      <x v="35"/>
-      <x v="35"/>
+      <x v="39"/>
+      <x v="39"/>
+    </i>
+    <i r="4">
+      <x v="40"/>
+      <x v="40"/>
+    </i>
+    <i t="grand">
+      <x/>
     </i>
   </rowItems>
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="2">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
   </colItems>
-  <dataFields count="3">
+  <pageFields count="2">
+    <pageField fld="10" hier="296" name="[Shared_DimTransactionDate].[YearNumber].&amp;[2010]" cap="2010"/>
+    <pageField fld="9" hier="286" name="[Shared_DimTransactionDate].[MonthName].&amp;[May]" cap="May"/>
+  </pageFields>
+  <dataFields count="2">
     <dataField fld="1" baseField="0" baseItem="1" numFmtId="4"/>
     <dataField fld="2" baseField="0" baseItem="1" numFmtId="4"/>
-    <dataField fld="3" baseField="0" baseItem="1" numFmtId="4"/>
   </dataFields>
-  <pivotHierarchies count="396">
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
+  <pivotHierarchies count="455">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy multipleItemSelectionAllowed="1"/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy multipleItemSelectionAllowed="1"/>
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -2427,8 +2781,14 @@
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy multipleItemSelectionAllowed="1">
-      <members count="1" level="1">
-        <member name="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2014]"/>
+      <members count="7" level="1">
+        <member name="[Shared_DimTransactionDate].[MonthName].&amp;[May]"/>
+        <member name="[Shared_DimTransactionDate].[MonthName].&amp;[July]"/>
+        <member name="[Shared_DimTransactionDate].[MonthName].&amp;[June]"/>
+        <member name="[Shared_DimTransactionDate].[MonthName].&amp;[April]"/>
+        <member name="[Shared_DimTransactionDate].[MonthName].&amp;[March]"/>
+        <member name="[Shared_DimTransactionDate].[MonthName].&amp;[January]"/>
+        <member name="[Shared_DimTransactionDate].[MonthName].&amp;[February]"/>
       </members>
     </pivotHierarchy>
     <pivotHierarchy/>
@@ -2440,116 +2800,135 @@
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
+    <pivotHierarchy multipleItemSelectionAllowed="1">
+      <members count="5" level="1">
+        <member name="[Shared_DimTransactionDate].[YearNumber].&amp;[2010]"/>
+        <member name="[Shared_DimTransactionDate].[YearNumber].&amp;[2011]"/>
+        <member name="[Shared_DimTransactionDate].[YearNumber].&amp;[2012]"/>
+        <member name="[Shared_DimTransactionDate].[YearNumber].&amp;[2013]"/>
+        <member name="[Shared_DimTransactionDate].[YearNumber].&amp;[2014]"/>
+      </members>
+    </pivotHierarchy>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
@@ -2591,12 +2970,12 @@
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="6">
-    <rowHierarchyUsage hierarchyUsage="83"/>
-    <rowHierarchyUsage hierarchyUsage="84"/>
-    <rowHierarchyUsage hierarchyUsage="85"/>
-    <rowHierarchyUsage hierarchyUsage="86"/>
-    <rowHierarchyUsage hierarchyUsage="82"/>
-    <rowHierarchyUsage hierarchyUsage="87"/>
+    <rowHierarchyUsage hierarchyUsage="144"/>
+    <rowHierarchyUsage hierarchyUsage="145"/>
+    <rowHierarchyUsage hierarchyUsage="146"/>
+    <rowHierarchyUsage hierarchyUsage="147"/>
+    <rowHierarchyUsage hierarchyUsage="143"/>
+    <rowHierarchyUsage hierarchyUsage="148"/>
   </rowHierarchiesUsage>
   <colHierarchiesUsage count="1">
     <colHierarchyUsage hierarchyUsage="-2"/>
@@ -2610,163 +2989,75 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Hierarchy1" sourceName="[Shared_DimTransactionDate].[Hierarchy1]">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_YearNumber" sourceName="[DatePeriodSelector].[YearNumber]">
   <pivotTables>
     <pivotTable tabId="1" name="PivotTable1"/>
   </pivotTables>
   <data>
-    <olap pivotCacheId="2">
-      <levels count="3">
-        <level uniqueName="[Shared_DimTransactionDate].[Hierarchy1].[(All)]" sourceCaption="(All)" count="0"/>
-        <level uniqueName="[Shared_DimTransactionDate].[Hierarchy1].[Year]" sourceCaption="Year" count="123">
+    <olap pivotCacheId="5">
+      <levels count="2">
+        <level uniqueName="[DatePeriodSelector].[YearNumber].[(All)]" sourceCaption="(All)" count="0"/>
+        <level uniqueName="[DatePeriodSelector].[YearNumber].[YearNumber]" sourceCaption="YearNumber" count="6">
           <ranges>
             <range startItem="0">
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2010]" c="2010"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2011]" c="2011"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2012]" c="2012"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2013]" c="2013"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2014]" c="2014"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2015]" c="2015"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;" c=""/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1899]" c="1899" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1900]" c="1900" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1901]" c="1901" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1902]" c="1902" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1903]" c="1903" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1904]" c="1904" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1905]" c="1905" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1906]" c="1906" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1907]" c="1907" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1908]" c="1908" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1909]" c="1909" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1910]" c="1910" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1911]" c="1911" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1912]" c="1912" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1913]" c="1913" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1914]" c="1914" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1915]" c="1915" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1916]" c="1916" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1917]" c="1917" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1918]" c="1918" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1919]" c="1919" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1920]" c="1920" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1921]" c="1921" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1922]" c="1922" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1923]" c="1923" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1924]" c="1924" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1925]" c="1925" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1926]" c="1926" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1927]" c="1927" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1928]" c="1928" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1929]" c="1929" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1930]" c="1930" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1931]" c="1931" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1932]" c="1932" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1933]" c="1933" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1934]" c="1934" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1935]" c="1935" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1936]" c="1936" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1937]" c="1937" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1938]" c="1938" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1939]" c="1939" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1940]" c="1940" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1941]" c="1941" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1942]" c="1942" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1943]" c="1943" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1944]" c="1944" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1945]" c="1945" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1946]" c="1946" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1947]" c="1947" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1948]" c="1948" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1949]" c="1949" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1950]" c="1950" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1951]" c="1951" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1952]" c="1952" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1953]" c="1953" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1954]" c="1954" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1955]" c="1955" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1956]" c="1956" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1957]" c="1957" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1958]" c="1958" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1959]" c="1959" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1960]" c="1960" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1961]" c="1961" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1962]" c="1962" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1963]" c="1963" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1964]" c="1964" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1965]" c="1965" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1966]" c="1966" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1967]" c="1967" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1968]" c="1968" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1969]" c="1969" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1970]" c="1970" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1971]" c="1971" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1972]" c="1972" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1973]" c="1973" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1974]" c="1974" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1975]" c="1975" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1976]" c="1976" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1977]" c="1977" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1978]" c="1978" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1979]" c="1979" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1980]" c="1980" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1981]" c="1981" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1982]" c="1982" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1983]" c="1983" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1984]" c="1984" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1985]" c="1985" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1986]" c="1986" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1987]" c="1987" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1988]" c="1988" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1989]" c="1989" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1990]" c="1990" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1991]" c="1991" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1992]" c="1992" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1993]" c="1993" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1994]" c="1994" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1995]" c="1995" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1996]" c="1996" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1997]" c="1997" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1998]" c="1998" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[1999]" c="1999" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2000]" c="2000" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2001]" c="2001" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2002]" c="2002" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2003]" c="2003" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2004]" c="2004" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2005]" c="2005" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2006]" c="2006" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2007]" c="2007" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2008]" c="2008" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2009]" c="2009" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2016]" c="2016" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2017]" c="2017" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2018]" c="2018" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2019]" c="2019" nd="1"/>
-              <i n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2020]" c="2020" nd="1"/>
+              <i n="[DatePeriodSelector].[YearNumber].&amp;[2010]" c="2010"/>
+              <i n="[DatePeriodSelector].[YearNumber].&amp;[2011]" c="2011"/>
+              <i n="[DatePeriodSelector].[YearNumber].&amp;[2012]" c="2012"/>
+              <i n="[DatePeriodSelector].[YearNumber].&amp;[2013]" c="2013"/>
+              <i n="[DatePeriodSelector].[YearNumber].&amp;[2014]" c="2014"/>
+              <i n="[DatePeriodSelector].[YearNumber].&amp;[2015]" c="2015" nd="1"/>
             </range>
           </ranges>
         </level>
-        <level uniqueName="[Shared_DimTransactionDate].[Hierarchy1].[MonthName]" sourceCaption="MonthName" count="0"/>
       </levels>
       <selections count="1">
-        <selection n="[Shared_DimTransactionDate].[Hierarchy1].[Year].&amp;[2014]"/>
+        <selection n="[DatePeriodSelector].[YearNumber].[All]"/>
       </selections>
     </olap>
   </data>
-  <extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{470722E0-AACD-4C17-9CDC-17EF765DBC7E}">
-      <x15:slicerCacheHideItemsWithNoData count="1">
-        <x15:slicerCacheOlapLevelName uniqueName="[Shared_DimTransactionDate].[Hierarchy1].[Year]" count="116"/>
-      </x15:slicerCacheHideItemsWithNoData>
-    </x:ext>
-  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_MonthName" sourceName="[DatePeriodSelector].[MonthName]">
+  <pivotTables>
+    <pivotTable tabId="1" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <olap pivotCacheId="5">
+      <levels count="2">
+        <level uniqueName="[DatePeriodSelector].[MonthName].[(All)]" sourceCaption="(All)" count="0"/>
+        <level uniqueName="[DatePeriodSelector].[MonthName].[MonthName]" sourceCaption="MonthName" count="12">
+          <ranges>
+            <range startItem="0">
+              <i n="[DatePeriodSelector].[MonthName].&amp;[January]" c="January"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[February]" c="February"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[March]" c="March"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[April]" c="April"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[May]" c="May"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[June]" c="June"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[July]" c="July"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[August]" c="August" nd="1"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[September]" c="September" nd="1"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[October]" c="October" nd="1"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[November]" c="November" nd="1"/>
+              <i n="[DatePeriodSelector].[MonthName].&amp;[December]" c="December" nd="1"/>
+            </range>
+          </ranges>
+        </level>
+      </levels>
+      <selections count="1">
+        <selection n="[DatePeriodSelector].[MonthName].[All]"/>
+      </selections>
+    </olap>
+  </data>
 </slicerCacheDefinition>
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Year" cache="Slicer_Hierarchy1" caption="Year" level="1" rowHeight="241300"/>
+  <slicer name="YearNumber" cache="Slicer_YearNumber" caption="YearNumber" level="1" rowHeight="241300"/>
+  <slicer name="MonthName" cache="Slicer_MonthName" caption="MonthName" level="1" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -3033,40 +3324,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:K46"/>
+  <dimension ref="D4:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D17" activeCellId="1" sqref="D9 D11:D34 D36:D51"/>
+      <pivotSelection pane="bottomRight" showHeader="1" dimension="1" activeRow="16" activeCol="3" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+          <references count="1">
+            <reference field="4" count="0"/>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.140625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="62.5703125" customWidth="1"/>
-    <col min="9" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s" vm="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" t="s" vm="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="I7" t="s">
         <v>1</v>
@@ -3074,701 +3388,662 @@
       <c r="J7" t="s">
         <v>2</v>
       </c>
-      <c r="K7" t="s">
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D8" s="2" t="s">
+      <c r="I8" s="4">
+        <v>90826913918.380005</v>
+      </c>
+      <c r="J8" s="4">
+        <v>91171371695.779984</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="4">
+        <v>90826913918.380005</v>
+      </c>
+      <c r="J9" s="4">
+        <v>91171371695.779984</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="4">
-        <v>85930966843.450012</v>
-      </c>
-      <c r="J8" s="4">
-        <v>86474080169.729965</v>
-      </c>
-      <c r="K8" s="4">
-        <v>-543113326.279953</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
+      <c r="I10" s="4">
+        <v>91663612471.76001</v>
+      </c>
+      <c r="J10" s="4">
+        <v>90920094187.650085</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="4">
-        <v>85930966843.449997</v>
-      </c>
-      <c r="J9" s="4">
-        <v>86474080169.72998</v>
-      </c>
-      <c r="K9" s="4">
-        <v>-543113326.27998352</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="4">
-        <v>88756549890.860031</v>
-      </c>
-      <c r="J10" s="4">
-        <v>87740139772.820007</v>
-      </c>
-      <c r="K10" s="4">
-        <v>1016410118.0400238</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I11" s="4">
-        <v>1297406217.3700001</v>
+        <v>901969492.54999995</v>
       </c>
       <c r="J11" s="4">
-        <v>1301999321.0200005</v>
-      </c>
-      <c r="K11" s="4">
-        <v>-4593103.6500003338</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+        <v>927507570.94000065</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
       <c r="G12" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I12" s="4">
-        <v>66440353532.330025</v>
+        <v>70117112435.800034</v>
       </c>
       <c r="J12" s="4">
-        <v>66144962617.500008</v>
-      </c>
-      <c r="K12" s="4">
-        <v>295390914.83001709</v>
-      </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+        <v>69928672065.260086</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
       <c r="G13" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="4">
-        <v>111601837.30999999</v>
+        <v>70898175.069999993</v>
       </c>
       <c r="J13" s="4">
-        <v>119030354.62</v>
-      </c>
-      <c r="K13" s="4">
-        <v>-7428517.3100000173</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+        <v>75371950.390000001</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
       <c r="G14" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="4">
-        <v>3133520</v>
+        <v>1348770</v>
       </c>
       <c r="J14" s="4">
-        <v>5096320</v>
-      </c>
-      <c r="K14" s="4">
-        <v>-1962800</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+        <v>4704340</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
       <c r="G15" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="4">
+        <v>27843.26</v>
+      </c>
+      <c r="J15" s="4">
+        <v>399469.9099999998</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="4">
+        <v>130433.46000000002</v>
+      </c>
+      <c r="J16" s="4">
+        <v>130433.45999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="4">
-        <v>121738</v>
-      </c>
-      <c r="J15" s="4">
-        <v>559612</v>
-      </c>
-      <c r="K15" s="4">
-        <v>-437874</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="I17" s="4">
+        <v>19606</v>
+      </c>
+      <c r="J17" s="4">
+        <v>247708</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="4">
-        <v>1850</v>
-      </c>
-      <c r="J16" s="4">
-        <v>100</v>
-      </c>
-      <c r="K16" s="4">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I17" s="4">
-        <v>95873258.340000004</v>
-      </c>
-      <c r="J17" s="4">
-        <v>74719048.340000004</v>
-      </c>
-      <c r="K17" s="4">
-        <v>21154210</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="I18" s="4">
-        <v>80498285.549999997</v>
+        <v>70900</v>
       </c>
       <c r="J18" s="4">
-        <v>84011584</v>
-      </c>
-      <c r="K18" s="4">
-        <v>-3513298.450000003</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+        <v>93050</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="4">
+        <v>9600</v>
+      </c>
+      <c r="J19" s="4">
+        <v>54603916.340000004</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" s="4">
+        <v>100611</v>
+      </c>
+      <c r="J20" s="4">
+        <v>3150000</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="4">
-        <v>1570801801</v>
-      </c>
-      <c r="J19" s="4">
-        <v>1312770110</v>
-      </c>
-      <c r="K19" s="4">
-        <v>258031691</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="I21" s="4">
+        <v>1207935311.75</v>
+      </c>
+      <c r="J21" s="4">
+        <v>938146164.99000001</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="4">
-        <v>213341615.5499998</v>
-      </c>
-      <c r="J20" s="4">
-        <v>155194850.05999997</v>
-      </c>
-      <c r="K20" s="4">
-        <v>58146765.489999831</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="2" t="s">
+      <c r="I22" s="4">
+        <v>155833354.62999988</v>
+      </c>
+      <c r="J22" s="4">
+        <v>155494059.88000003</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="4">
+        <v>18357919224.430004</v>
+      </c>
+      <c r="J23" s="4">
+        <v>18001056555.590004</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="4">
-        <v>17868424991.770004</v>
-      </c>
-      <c r="J21" s="4">
-        <v>17472802573.220005</v>
-      </c>
-      <c r="K21" s="4">
-        <v>395622418.54999924</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="2" t="s">
+      <c r="I24" s="4">
+        <v>36819900</v>
+      </c>
+      <c r="J24" s="4">
+        <v>32549079.749999996</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="4">
+        <v>61559569.960000031</v>
+      </c>
+      <c r="J25" s="4">
+        <v>58382335.770000011</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="4">
+        <v>751549272.53000021</v>
+      </c>
+      <c r="J26" s="4">
+        <v>738751819.34000015</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>2753.75</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="4">
-        <v>74643440</v>
-      </c>
-      <c r="J22" s="4">
-        <v>74070406.839999989</v>
-      </c>
-      <c r="K22" s="4">
-        <v>573033.16000001132</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="I23" s="4">
-        <v>69574120.75</v>
-      </c>
-      <c r="J23" s="4">
-        <v>65901056.310000069</v>
-      </c>
-      <c r="K23" s="4">
-        <v>3673064.4399999306</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24" s="4">
-        <v>929556812.89000046</v>
-      </c>
-      <c r="J24" s="4">
-        <v>927798572.19999921</v>
-      </c>
-      <c r="K24" s="4">
-        <v>1758240.6900012493</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0</v>
-      </c>
-      <c r="J25" s="4">
-        <v>25</v>
-      </c>
-      <c r="K25" s="4">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0</v>
-      </c>
-      <c r="J26" s="4">
-        <v>1300</v>
-      </c>
-      <c r="K26" s="4">
-        <v>-1300</v>
-      </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="4">
-        <v>1216870</v>
-      </c>
-      <c r="J27" s="4">
-        <v>1205690</v>
-      </c>
-      <c r="K27" s="4">
-        <v>11180</v>
-      </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I28" s="4">
         <v>0</v>
       </c>
       <c r="J28" s="4">
-        <v>-1506.29</v>
-      </c>
-      <c r="K28" s="4">
-        <v>1506.29</v>
-      </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+        <v>16350.150000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="G29" s="2" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="I29" s="4">
         <v>0</v>
       </c>
       <c r="J29" s="4">
-        <v>17738</v>
-      </c>
-      <c r="K29" s="4">
-        <v>-17738</v>
-      </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+        <v>285.75000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="G30" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I30" s="4">
+        <v>164810</v>
+      </c>
+      <c r="J30" s="4">
+        <v>623733.62</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" s="4">
+        <v>500</v>
+      </c>
+      <c r="J31" s="4">
+        <v>43062.150000000023</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="4">
         <v>0</v>
       </c>
-      <c r="J30" s="4">
-        <v>0</v>
-      </c>
-      <c r="K30" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I31" s="4">
-        <v>11462616634.909998</v>
-      </c>
-      <c r="J31" s="4">
-        <v>11935568987.050003</v>
-      </c>
-      <c r="K31" s="4">
-        <v>-472952352.14000511</v>
-      </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" s="4">
-        <v>4623120</v>
-      </c>
       <c r="J32" s="4">
-        <v>2226380</v>
-      </c>
-      <c r="K32" s="4">
-        <v>2396740</v>
-      </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+        <v>9174.15</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
       <c r="G33" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="I33" s="4">
-        <v>454350</v>
+        <v>130433.45999999999</v>
       </c>
       <c r="J33" s="4">
-        <v>256300</v>
-      </c>
-      <c r="K33" s="4">
-        <v>198050</v>
-      </c>
-    </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+        <v>130433.45999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
       <c r="G34" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="I34" s="4">
-        <v>487990</v>
+        <v>12227.86</v>
       </c>
       <c r="J34" s="4">
-        <v>437930</v>
-      </c>
-      <c r="K34" s="4">
-        <v>50060</v>
-      </c>
-    </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>46</v>
+        <v>7875</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="I35" s="4">
-        <v>5400</v>
+        <v>16664408409.43</v>
       </c>
       <c r="J35" s="4">
-        <v>5840</v>
-      </c>
-      <c r="K35" s="4">
-        <v>-440</v>
-      </c>
-    </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+        <v>17063108915.629999</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="G36" s="2" t="s">
         <v>75</v>
       </c>
       <c r="H36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2028080</v>
+      </c>
+      <c r="J36" s="4">
+        <v>741320</v>
+      </c>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" s="4">
+        <v>2782380</v>
+      </c>
+      <c r="J37" s="4">
+        <v>509150</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" s="4">
+        <v>444880</v>
+      </c>
+      <c r="J38" s="4">
+        <v>396880</v>
+      </c>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I39" s="4">
+        <v>5180</v>
+      </c>
+      <c r="J39" s="4">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I40" s="4">
+        <v>988304.90000000026</v>
+      </c>
+      <c r="J40" s="4">
+        <v>3841793.5599999996</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I36" s="4">
-        <v>1725316.8600000003</v>
-      </c>
-      <c r="J36" s="4">
-        <v>3000000</v>
-      </c>
-      <c r="K36" s="4">
-        <v>-1274683.1399999997</v>
-      </c>
-    </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="I41" s="4">
+        <v>420</v>
+      </c>
+      <c r="J41" s="4">
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="4">
+        <v>982730</v>
+      </c>
+      <c r="J42" s="4">
+        <v>1732290</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I43" s="4">
+        <v>115474.82</v>
+      </c>
+      <c r="J43" s="4">
+        <v>122092.51</v>
+      </c>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I44" s="4">
+        <v>133128</v>
+      </c>
+      <c r="J44" s="4">
+        <v>93157</v>
+      </c>
+    </row>
+    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" s="4">
+        <v>3999708.3199999994</v>
+      </c>
+      <c r="J45" s="4">
         <v>0</v>
       </c>
-      <c r="J37" s="4">
-        <v>0</v>
-      </c>
-      <c r="K37" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G38" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H38" s="2" t="s">
+    </row>
+    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G46" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I46" s="4">
+        <v>14710.81</v>
+      </c>
+      <c r="J46" s="4">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I47" s="4">
+        <v>114580</v>
+      </c>
+      <c r="J47" s="4">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I48" s="4">
+        <v>3150000</v>
+      </c>
+      <c r="J48" s="4">
+        <v>100611</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I49" s="4">
+        <v>16603444839.92</v>
+      </c>
+      <c r="J49" s="4">
+        <v>17055126651.700001</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I50" s="4">
+        <v>46073559.199999988</v>
+      </c>
+      <c r="J50" s="4">
+        <v>297806.40000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I38" s="4">
-        <v>0</v>
-      </c>
-      <c r="J38" s="4">
-        <v>0</v>
-      </c>
-      <c r="K38" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G39" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="4">
-        <v>0</v>
-      </c>
-      <c r="J39" s="4">
-        <v>0</v>
-      </c>
-      <c r="K39" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G40" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I40" s="4">
-        <v>441037</v>
-      </c>
-      <c r="J40" s="4">
-        <v>195204</v>
-      </c>
-      <c r="K40" s="4">
-        <v>245833</v>
-      </c>
-    </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G41" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I41" s="4">
-        <v>10733169.030000003</v>
-      </c>
-      <c r="J41" s="4">
-        <v>27.47</v>
-      </c>
-      <c r="K41" s="4">
-        <v>10733141.560000002</v>
-      </c>
-    </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G42" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I42" s="4">
-        <v>21073.46</v>
-      </c>
-      <c r="J42" s="4">
-        <v>2400</v>
-      </c>
-      <c r="K42" s="4">
-        <v>18673.46</v>
-      </c>
-    </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G43" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I43" s="4">
-        <v>118575</v>
-      </c>
-      <c r="J43" s="4">
-        <v>2635</v>
-      </c>
-      <c r="K43" s="4">
-        <v>115940</v>
-      </c>
-    </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I44" s="4">
-        <v>84011584</v>
-      </c>
-      <c r="J44" s="4">
-        <v>80498285.549999997</v>
-      </c>
-      <c r="K44" s="4">
-        <v>3513298.450000003</v>
-      </c>
-    </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E45" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I45" s="4">
-        <v>11289106511.26</v>
-      </c>
-      <c r="J45" s="4">
-        <v>11759548333.530001</v>
-      </c>
-      <c r="K45" s="4">
-        <v>-470441822.27000046</v>
-      </c>
-    </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="G46" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I46" s="4">
-        <v>70888508.300000012</v>
-      </c>
-      <c r="J46" s="4">
-        <v>89395651.500000045</v>
-      </c>
-      <c r="K46" s="4">
-        <v>-18507143.200000033</v>
+      <c r="I51" s="4">
+        <v>130433.46000000002</v>
+      </c>
+      <c r="J51" s="4">
+        <v>130433.45999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I52" s="4">
+        <v>199154934799.5701</v>
+      </c>
+      <c r="J52" s="4">
+        <v>199154574799.05997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>